<commit_message>
Multiprocessing, take params from train_params.xlsx, output an xlsx file for each trial, insert all results to a single table in the database
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C664C0A4-98F9-C04A-91C7-E25CFD756E2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDA7507-117D-B344-BED6-765D51E72937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -52,10 +52,10 @@
     <t>topn</t>
   </si>
   <si>
-    <t>data_words</t>
-  </si>
-  <si>
     <t>qa</t>
+  </si>
+  <si>
+    <t>data_words_type</t>
   </si>
 </sst>
 </file>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -420,7 +420,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -479,6 +479,102 @@
         <v>2</v>
       </c>
       <c r="J2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.25</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5">
+        <v>0.25</v>
+      </c>
+      <c r="G5">
+        <v>0.25</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
train_params remembers that eta can only be "auto" now
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDA7507-117D-B344-BED6-765D51E72937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8973F-9055-FA45-AFD1-0AC59D300D18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A4" sqref="A4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,70 +514,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.1</v>
-      </c>
-      <c r="F4">
-        <v>0.25</v>
-      </c>
-      <c r="G4">
-        <v>0.25</v>
-      </c>
-      <c r="H4">
-        <v>1000</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>40</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <v>0.25</v>
-      </c>
-      <c r="G5">
-        <v>0.25</v>
-      </c>
-      <c r="H5">
-        <v>1000</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Store data_lemmatized, corpus and id2word to prevent recalculations, which are very expensive.
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8973F-9055-FA45-AFD1-0AC59D300D18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F879EF-6D76-6E48-9BBC-82ADB0AD860B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J5"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,6 +514,1030 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.1</v>
+      </c>
+      <c r="F4">
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0.1</v>
+      </c>
+      <c r="F5">
+        <v>0.25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>43</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+      <c r="F6">
+        <v>0.25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>44</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0.25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>0.25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0.25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>48</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11">
+        <v>0.25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>49</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <v>0.25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>0.25</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>41</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.2</v>
+      </c>
+      <c r="F15">
+        <v>0.25</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1000</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>42</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.2</v>
+      </c>
+      <c r="F16">
+        <v>0.25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1000</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>43</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.2</v>
+      </c>
+      <c r="F17">
+        <v>0.25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1000</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.2</v>
+      </c>
+      <c r="F18">
+        <v>0.25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1000</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0.2</v>
+      </c>
+      <c r="F19">
+        <v>0.25</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1000</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>46</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>0.25</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1000</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>47</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0.2</v>
+      </c>
+      <c r="F21">
+        <v>0.25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1000</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>48</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>0.25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1000</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>49</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0.2</v>
+      </c>
+      <c r="F23">
+        <v>0.25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1000</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0.2</v>
+      </c>
+      <c r="F24">
+        <v>0.25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1000</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.2</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1000</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>41</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0.2</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1000</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>42</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0.2</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1000</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>43</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0.2</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1000</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>44</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0.2</v>
+      </c>
+      <c r="F29">
+        <v>0.1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1000</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>45</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0.2</v>
+      </c>
+      <c r="F30">
+        <v>0.1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1000</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>46</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.2</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1000</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>47</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0.2</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1000</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>48</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0.2</v>
+      </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1000</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>49</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0.2</v>
+      </c>
+      <c r="F34">
+        <v>0.1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1000</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0.2</v>
+      </c>
+      <c r="F35">
+        <v>0.1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1000</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Rearrange cells of output excel file. Trained 36.
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F879EF-6D76-6E48-9BBC-82ADB0AD860B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96364C0-6151-4649-BC6B-449530DB5B02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1538,6 +1538,230 @@
         <v>20</v>
       </c>
     </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>50</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0.2</v>
+      </c>
+      <c r="F36">
+        <v>0.1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1000</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>50</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0.2</v>
+      </c>
+      <c r="F37">
+        <v>0.1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>1000</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>50</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0.3</v>
+      </c>
+      <c r="F38">
+        <v>0.1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>1000</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>50</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0.4</v>
+      </c>
+      <c r="F39">
+        <v>0.1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1000</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>50</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <v>0.1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1000</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>50</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0.6</v>
+      </c>
+      <c r="F41">
+        <v>0.1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1000</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>50</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0.7</v>
+      </c>
+      <c r="F42">
+        <v>0.1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1000</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed 41. Train row 42 to 191.
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96364C0-6151-4649-BC6B-449530DB5B02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14E1D8-8FE0-8347-8FF8-45323D877587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="L191" sqref="L191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1762,6 +1762,4806 @@
         <v>20</v>
       </c>
     </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>51</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.5</v>
+      </c>
+      <c r="F43">
+        <v>0.1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>1000</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>52</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0.5</v>
+      </c>
+      <c r="F44">
+        <v>0.1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>1000</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>53</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.5</v>
+      </c>
+      <c r="F45">
+        <v>0.1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>1000</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>54</v>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0.5</v>
+      </c>
+      <c r="F46">
+        <v>0.1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>1000</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>55</v>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+      <c r="F47">
+        <v>0.1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>1000</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>56</v>
+      </c>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0.5</v>
+      </c>
+      <c r="F48">
+        <v>0.1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>1000</v>
+      </c>
+      <c r="I48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>57</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0.5</v>
+      </c>
+      <c r="F49">
+        <v>0.1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1000</v>
+      </c>
+      <c r="I49">
+        <v>2</v>
+      </c>
+      <c r="J49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>58</v>
+      </c>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0.5</v>
+      </c>
+      <c r="F50">
+        <v>0.1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>1000</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>59</v>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0.5</v>
+      </c>
+      <c r="F51">
+        <v>0.1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1000</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>60</v>
+      </c>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0.5</v>
+      </c>
+      <c r="F52">
+        <v>0.1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>1000</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>61</v>
+      </c>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.5</v>
+      </c>
+      <c r="F53">
+        <v>0.1</v>
+      </c>
+      <c r="G53" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>1000</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54">
+        <v>62</v>
+      </c>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0.5</v>
+      </c>
+      <c r="F54">
+        <v>0.1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>1000</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>63</v>
+      </c>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0.5</v>
+      </c>
+      <c r="F55">
+        <v>0.1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>1000</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>64</v>
+      </c>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="F56">
+        <v>0.1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>1000</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>65</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+      <c r="F57">
+        <v>0.1</v>
+      </c>
+      <c r="G57" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>1000</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>66</v>
+      </c>
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.5</v>
+      </c>
+      <c r="F58">
+        <v>0.1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>1000</v>
+      </c>
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>67</v>
+      </c>
+      <c r="C59" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0.5</v>
+      </c>
+      <c r="F59">
+        <v>0.1</v>
+      </c>
+      <c r="G59" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>1000</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>68</v>
+      </c>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0.5</v>
+      </c>
+      <c r="F60">
+        <v>0.1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>1000</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>69</v>
+      </c>
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0.5</v>
+      </c>
+      <c r="F61">
+        <v>0.1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1000</v>
+      </c>
+      <c r="I61">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>70</v>
+      </c>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0.5</v>
+      </c>
+      <c r="F62">
+        <v>0.1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>1000</v>
+      </c>
+      <c r="I62">
+        <v>2</v>
+      </c>
+      <c r="J62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>71</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0.5</v>
+      </c>
+      <c r="F63">
+        <v>0.1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1000</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64">
+        <v>72</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0.5</v>
+      </c>
+      <c r="F64">
+        <v>0.1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1000</v>
+      </c>
+      <c r="I64">
+        <v>2</v>
+      </c>
+      <c r="J64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>73</v>
+      </c>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0.5</v>
+      </c>
+      <c r="F65">
+        <v>0.1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>1000</v>
+      </c>
+      <c r="I65">
+        <v>2</v>
+      </c>
+      <c r="J65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>74</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0.5</v>
+      </c>
+      <c r="F66">
+        <v>0.1</v>
+      </c>
+      <c r="G66" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>1000</v>
+      </c>
+      <c r="I66">
+        <v>2</v>
+      </c>
+      <c r="J66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>75</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0.5</v>
+      </c>
+      <c r="F67">
+        <v>0.1</v>
+      </c>
+      <c r="G67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>1000</v>
+      </c>
+      <c r="I67">
+        <v>2</v>
+      </c>
+      <c r="J67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>76</v>
+      </c>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0.5</v>
+      </c>
+      <c r="F68">
+        <v>0.1</v>
+      </c>
+      <c r="G68" t="s">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>1000</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+      <c r="J68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>77</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0.5</v>
+      </c>
+      <c r="F69">
+        <v>0.1</v>
+      </c>
+      <c r="G69" t="s">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>1000</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>78</v>
+      </c>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0.5</v>
+      </c>
+      <c r="F70">
+        <v>0.1</v>
+      </c>
+      <c r="G70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>1000</v>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+      <c r="J70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>79</v>
+      </c>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0.5</v>
+      </c>
+      <c r="F71">
+        <v>0.1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>1000</v>
+      </c>
+      <c r="I71">
+        <v>2</v>
+      </c>
+      <c r="J71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72">
+        <v>80</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0.5</v>
+      </c>
+      <c r="F72">
+        <v>0.1</v>
+      </c>
+      <c r="G72" t="s">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>1000</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>81</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0.5</v>
+      </c>
+      <c r="F73">
+        <v>0.1</v>
+      </c>
+      <c r="G73" t="s">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>1000</v>
+      </c>
+      <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74">
+        <v>82</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0.5</v>
+      </c>
+      <c r="F74">
+        <v>0.1</v>
+      </c>
+      <c r="G74" t="s">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>1000</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>83</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0.5</v>
+      </c>
+      <c r="F75">
+        <v>0.1</v>
+      </c>
+      <c r="G75" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>1000</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+      <c r="J75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>84</v>
+      </c>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0.5</v>
+      </c>
+      <c r="F76">
+        <v>0.1</v>
+      </c>
+      <c r="G76" t="s">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>1000</v>
+      </c>
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77">
+        <v>85</v>
+      </c>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0.5</v>
+      </c>
+      <c r="F77">
+        <v>0.1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>1000</v>
+      </c>
+      <c r="I77">
+        <v>2</v>
+      </c>
+      <c r="J77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78">
+        <v>86</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0.5</v>
+      </c>
+      <c r="F78">
+        <v>0.1</v>
+      </c>
+      <c r="G78" t="s">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>1000</v>
+      </c>
+      <c r="I78">
+        <v>2</v>
+      </c>
+      <c r="J78">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79">
+        <v>87</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0.5</v>
+      </c>
+      <c r="F79">
+        <v>0.1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>1000</v>
+      </c>
+      <c r="I79">
+        <v>2</v>
+      </c>
+      <c r="J79">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80">
+        <v>88</v>
+      </c>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0.5</v>
+      </c>
+      <c r="F80">
+        <v>0.1</v>
+      </c>
+      <c r="G80" t="s">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>1000</v>
+      </c>
+      <c r="I80">
+        <v>2</v>
+      </c>
+      <c r="J80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81">
+        <v>89</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0.5</v>
+      </c>
+      <c r="F81">
+        <v>0.1</v>
+      </c>
+      <c r="G81" t="s">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>1000</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+      <c r="J81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82">
+        <v>90</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0.5</v>
+      </c>
+      <c r="F82">
+        <v>0.1</v>
+      </c>
+      <c r="G82" t="s">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>1000</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83">
+        <v>91</v>
+      </c>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0.5</v>
+      </c>
+      <c r="F83">
+        <v>0.1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>1000</v>
+      </c>
+      <c r="I83">
+        <v>2</v>
+      </c>
+      <c r="J83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84">
+        <v>92</v>
+      </c>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0.5</v>
+      </c>
+      <c r="F84">
+        <v>0.1</v>
+      </c>
+      <c r="G84" t="s">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>1000</v>
+      </c>
+      <c r="I84">
+        <v>2</v>
+      </c>
+      <c r="J84">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85">
+        <v>93</v>
+      </c>
+      <c r="C85" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0.5</v>
+      </c>
+      <c r="F85">
+        <v>0.1</v>
+      </c>
+      <c r="G85" t="s">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>1000</v>
+      </c>
+      <c r="I85">
+        <v>2</v>
+      </c>
+      <c r="J85">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>10</v>
+      </c>
+      <c r="B86">
+        <v>94</v>
+      </c>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0.5</v>
+      </c>
+      <c r="F86">
+        <v>0.1</v>
+      </c>
+      <c r="G86" t="s">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>1000</v>
+      </c>
+      <c r="I86">
+        <v>2</v>
+      </c>
+      <c r="J86">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>10</v>
+      </c>
+      <c r="B87">
+        <v>95</v>
+      </c>
+      <c r="C87" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0.5</v>
+      </c>
+      <c r="F87">
+        <v>0.1</v>
+      </c>
+      <c r="G87" t="s">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>1000</v>
+      </c>
+      <c r="I87">
+        <v>2</v>
+      </c>
+      <c r="J87">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>96</v>
+      </c>
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0.5</v>
+      </c>
+      <c r="F88">
+        <v>0.1</v>
+      </c>
+      <c r="G88" t="s">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>1000</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
+      <c r="J88">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>10</v>
+      </c>
+      <c r="B89">
+        <v>97</v>
+      </c>
+      <c r="C89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0.5</v>
+      </c>
+      <c r="F89">
+        <v>0.1</v>
+      </c>
+      <c r="G89" t="s">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>1000</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90">
+        <v>98</v>
+      </c>
+      <c r="C90" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0.5</v>
+      </c>
+      <c r="F90">
+        <v>0.1</v>
+      </c>
+      <c r="G90" t="s">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>1000</v>
+      </c>
+      <c r="I90">
+        <v>2</v>
+      </c>
+      <c r="J90">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>10</v>
+      </c>
+      <c r="B91">
+        <v>99</v>
+      </c>
+      <c r="C91" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0.5</v>
+      </c>
+      <c r="F91">
+        <v>0.1</v>
+      </c>
+      <c r="G91" t="s">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>1000</v>
+      </c>
+      <c r="I91">
+        <v>2</v>
+      </c>
+      <c r="J91">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92">
+        <v>100</v>
+      </c>
+      <c r="C92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0.5</v>
+      </c>
+      <c r="F92">
+        <v>0.1</v>
+      </c>
+      <c r="G92" t="s">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>1000</v>
+      </c>
+      <c r="I92">
+        <v>2</v>
+      </c>
+      <c r="J92">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93">
+        <v>101</v>
+      </c>
+      <c r="C93" t="b">
+        <v>1</v>
+      </c>
+      <c r="D93" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0.5</v>
+      </c>
+      <c r="F93">
+        <v>0.1</v>
+      </c>
+      <c r="G93" t="s">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>1000</v>
+      </c>
+      <c r="I93">
+        <v>2</v>
+      </c>
+      <c r="J93">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94">
+        <v>102</v>
+      </c>
+      <c r="C94" t="b">
+        <v>1</v>
+      </c>
+      <c r="D94" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0.5</v>
+      </c>
+      <c r="F94">
+        <v>0.1</v>
+      </c>
+      <c r="G94" t="s">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>1000</v>
+      </c>
+      <c r="I94">
+        <v>2</v>
+      </c>
+      <c r="J94">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95">
+        <v>103</v>
+      </c>
+      <c r="C95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0.5</v>
+      </c>
+      <c r="F95">
+        <v>0.1</v>
+      </c>
+      <c r="G95" t="s">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>1000</v>
+      </c>
+      <c r="I95">
+        <v>2</v>
+      </c>
+      <c r="J95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96">
+        <v>104</v>
+      </c>
+      <c r="C96" t="b">
+        <v>1</v>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0.5</v>
+      </c>
+      <c r="F96">
+        <v>0.1</v>
+      </c>
+      <c r="G96" t="s">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>1000</v>
+      </c>
+      <c r="I96">
+        <v>2</v>
+      </c>
+      <c r="J96">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97">
+        <v>105</v>
+      </c>
+      <c r="C97" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0.5</v>
+      </c>
+      <c r="F97">
+        <v>0.1</v>
+      </c>
+      <c r="G97" t="s">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>1000</v>
+      </c>
+      <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98">
+        <v>106</v>
+      </c>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0.5</v>
+      </c>
+      <c r="F98">
+        <v>0.1</v>
+      </c>
+      <c r="G98" t="s">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>1000</v>
+      </c>
+      <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="J98">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99">
+        <v>107</v>
+      </c>
+      <c r="C99" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0.5</v>
+      </c>
+      <c r="F99">
+        <v>0.1</v>
+      </c>
+      <c r="G99" t="s">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>1000</v>
+      </c>
+      <c r="I99">
+        <v>2</v>
+      </c>
+      <c r="J99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100">
+        <v>108</v>
+      </c>
+      <c r="C100" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0.5</v>
+      </c>
+      <c r="F100">
+        <v>0.1</v>
+      </c>
+      <c r="G100" t="s">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>1000</v>
+      </c>
+      <c r="I100">
+        <v>2</v>
+      </c>
+      <c r="J100">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101">
+        <v>109</v>
+      </c>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0.5</v>
+      </c>
+      <c r="F101">
+        <v>0.1</v>
+      </c>
+      <c r="G101" t="s">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>1000</v>
+      </c>
+      <c r="I101">
+        <v>2</v>
+      </c>
+      <c r="J101">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102">
+        <v>110</v>
+      </c>
+      <c r="C102" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0.5</v>
+      </c>
+      <c r="F102">
+        <v>0.1</v>
+      </c>
+      <c r="G102" t="s">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>1000</v>
+      </c>
+      <c r="I102">
+        <v>2</v>
+      </c>
+      <c r="J102">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103">
+        <v>111</v>
+      </c>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0.5</v>
+      </c>
+      <c r="F103">
+        <v>0.1</v>
+      </c>
+      <c r="G103" t="s">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>1000</v>
+      </c>
+      <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="J103">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104">
+        <v>112</v>
+      </c>
+      <c r="C104" t="b">
+        <v>1</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0.5</v>
+      </c>
+      <c r="F104">
+        <v>0.1</v>
+      </c>
+      <c r="G104" t="s">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>1000</v>
+      </c>
+      <c r="I104">
+        <v>2</v>
+      </c>
+      <c r="J104">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>10</v>
+      </c>
+      <c r="B105">
+        <v>113</v>
+      </c>
+      <c r="C105" t="b">
+        <v>1</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0.5</v>
+      </c>
+      <c r="F105">
+        <v>0.1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>1000</v>
+      </c>
+      <c r="I105">
+        <v>2</v>
+      </c>
+      <c r="J105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>10</v>
+      </c>
+      <c r="B106">
+        <v>114</v>
+      </c>
+      <c r="C106" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0.5</v>
+      </c>
+      <c r="F106">
+        <v>0.1</v>
+      </c>
+      <c r="G106" t="s">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>1000</v>
+      </c>
+      <c r="I106">
+        <v>2</v>
+      </c>
+      <c r="J106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>10</v>
+      </c>
+      <c r="B107">
+        <v>115</v>
+      </c>
+      <c r="C107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0.5</v>
+      </c>
+      <c r="F107">
+        <v>0.1</v>
+      </c>
+      <c r="G107" t="s">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>1000</v>
+      </c>
+      <c r="I107">
+        <v>2</v>
+      </c>
+      <c r="J107">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>10</v>
+      </c>
+      <c r="B108">
+        <v>116</v>
+      </c>
+      <c r="C108" t="b">
+        <v>1</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0.5</v>
+      </c>
+      <c r="F108">
+        <v>0.1</v>
+      </c>
+      <c r="G108" t="s">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>1000</v>
+      </c>
+      <c r="I108">
+        <v>2</v>
+      </c>
+      <c r="J108">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109">
+        <v>117</v>
+      </c>
+      <c r="C109" t="b">
+        <v>1</v>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0.5</v>
+      </c>
+      <c r="F109">
+        <v>0.1</v>
+      </c>
+      <c r="G109" t="s">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>1000</v>
+      </c>
+      <c r="I109">
+        <v>2</v>
+      </c>
+      <c r="J109">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110">
+        <v>118</v>
+      </c>
+      <c r="C110" t="b">
+        <v>1</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0.5</v>
+      </c>
+      <c r="F110">
+        <v>0.1</v>
+      </c>
+      <c r="G110" t="s">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>1000</v>
+      </c>
+      <c r="I110">
+        <v>2</v>
+      </c>
+      <c r="J110">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>10</v>
+      </c>
+      <c r="B111">
+        <v>119</v>
+      </c>
+      <c r="C111" t="b">
+        <v>1</v>
+      </c>
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0.5</v>
+      </c>
+      <c r="F111">
+        <v>0.1</v>
+      </c>
+      <c r="G111" t="s">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>1000</v>
+      </c>
+      <c r="I111">
+        <v>2</v>
+      </c>
+      <c r="J111">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>10</v>
+      </c>
+      <c r="B112">
+        <v>120</v>
+      </c>
+      <c r="C112" t="b">
+        <v>1</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0.5</v>
+      </c>
+      <c r="F112">
+        <v>0.1</v>
+      </c>
+      <c r="G112" t="s">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>1000</v>
+      </c>
+      <c r="I112">
+        <v>2</v>
+      </c>
+      <c r="J112">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>10</v>
+      </c>
+      <c r="B113">
+        <v>121</v>
+      </c>
+      <c r="C113" t="b">
+        <v>1</v>
+      </c>
+      <c r="D113" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0.5</v>
+      </c>
+      <c r="F113">
+        <v>0.1</v>
+      </c>
+      <c r="G113" t="s">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>1000</v>
+      </c>
+      <c r="I113">
+        <v>2</v>
+      </c>
+      <c r="J113">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>10</v>
+      </c>
+      <c r="B114">
+        <v>122</v>
+      </c>
+      <c r="C114" t="b">
+        <v>1</v>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0.5</v>
+      </c>
+      <c r="F114">
+        <v>0.1</v>
+      </c>
+      <c r="G114" t="s">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>1000</v>
+      </c>
+      <c r="I114">
+        <v>2</v>
+      </c>
+      <c r="J114">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>10</v>
+      </c>
+      <c r="B115">
+        <v>123</v>
+      </c>
+      <c r="C115" t="b">
+        <v>1</v>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0.5</v>
+      </c>
+      <c r="F115">
+        <v>0.1</v>
+      </c>
+      <c r="G115" t="s">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>1000</v>
+      </c>
+      <c r="I115">
+        <v>2</v>
+      </c>
+      <c r="J115">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>10</v>
+      </c>
+      <c r="B116">
+        <v>124</v>
+      </c>
+      <c r="C116" t="b">
+        <v>1</v>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0.5</v>
+      </c>
+      <c r="F116">
+        <v>0.1</v>
+      </c>
+      <c r="G116" t="s">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>1000</v>
+      </c>
+      <c r="I116">
+        <v>2</v>
+      </c>
+      <c r="J116">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117">
+        <v>125</v>
+      </c>
+      <c r="C117" t="b">
+        <v>1</v>
+      </c>
+      <c r="D117" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>0.5</v>
+      </c>
+      <c r="F117">
+        <v>0.1</v>
+      </c>
+      <c r="G117" t="s">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>1000</v>
+      </c>
+      <c r="I117">
+        <v>2</v>
+      </c>
+      <c r="J117">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118">
+        <v>51</v>
+      </c>
+      <c r="C118" t="b">
+        <v>1</v>
+      </c>
+      <c r="D118" t="b">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0.5</v>
+      </c>
+      <c r="F118">
+        <v>0.05</v>
+      </c>
+      <c r="G118" t="s">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>1000</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+      <c r="J118">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>10</v>
+      </c>
+      <c r="B119">
+        <v>52</v>
+      </c>
+      <c r="C119" t="b">
+        <v>1</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0.5</v>
+      </c>
+      <c r="F119">
+        <v>0.05</v>
+      </c>
+      <c r="G119" t="s">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>1000</v>
+      </c>
+      <c r="I119">
+        <v>2</v>
+      </c>
+      <c r="J119">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120">
+        <v>53</v>
+      </c>
+      <c r="C120" t="b">
+        <v>1</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0.5</v>
+      </c>
+      <c r="F120">
+        <v>0.05</v>
+      </c>
+      <c r="G120" t="s">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>1000</v>
+      </c>
+      <c r="I120">
+        <v>2</v>
+      </c>
+      <c r="J120">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>10</v>
+      </c>
+      <c r="B121">
+        <v>54</v>
+      </c>
+      <c r="C121" t="b">
+        <v>1</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <v>0.5</v>
+      </c>
+      <c r="F121">
+        <v>0.05</v>
+      </c>
+      <c r="G121" t="s">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>1000</v>
+      </c>
+      <c r="I121">
+        <v>2</v>
+      </c>
+      <c r="J121">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122">
+        <v>55</v>
+      </c>
+      <c r="C122" t="b">
+        <v>1</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0.5</v>
+      </c>
+      <c r="F122">
+        <v>0.05</v>
+      </c>
+      <c r="G122" t="s">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>1000</v>
+      </c>
+      <c r="I122">
+        <v>2</v>
+      </c>
+      <c r="J122">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>10</v>
+      </c>
+      <c r="B123">
+        <v>56</v>
+      </c>
+      <c r="C123" t="b">
+        <v>1</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0.5</v>
+      </c>
+      <c r="F123">
+        <v>0.05</v>
+      </c>
+      <c r="G123" t="s">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>1000</v>
+      </c>
+      <c r="I123">
+        <v>2</v>
+      </c>
+      <c r="J123">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>10</v>
+      </c>
+      <c r="B124">
+        <v>57</v>
+      </c>
+      <c r="C124" t="b">
+        <v>1</v>
+      </c>
+      <c r="D124" t="b">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>0.5</v>
+      </c>
+      <c r="F124">
+        <v>0.05</v>
+      </c>
+      <c r="G124" t="s">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>1000</v>
+      </c>
+      <c r="I124">
+        <v>2</v>
+      </c>
+      <c r="J124">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>10</v>
+      </c>
+      <c r="B125">
+        <v>58</v>
+      </c>
+      <c r="C125" t="b">
+        <v>1</v>
+      </c>
+      <c r="D125" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0.5</v>
+      </c>
+      <c r="F125">
+        <v>0.05</v>
+      </c>
+      <c r="G125" t="s">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>1000</v>
+      </c>
+      <c r="I125">
+        <v>2</v>
+      </c>
+      <c r="J125">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>10</v>
+      </c>
+      <c r="B126">
+        <v>59</v>
+      </c>
+      <c r="C126" t="b">
+        <v>1</v>
+      </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126">
+        <v>0.5</v>
+      </c>
+      <c r="F126">
+        <v>0.05</v>
+      </c>
+      <c r="G126" t="s">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>1000</v>
+      </c>
+      <c r="I126">
+        <v>2</v>
+      </c>
+      <c r="J126">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127">
+        <v>60</v>
+      </c>
+      <c r="C127" t="b">
+        <v>1</v>
+      </c>
+      <c r="D127" t="b">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0.5</v>
+      </c>
+      <c r="F127">
+        <v>0.05</v>
+      </c>
+      <c r="G127" t="s">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>1000</v>
+      </c>
+      <c r="I127">
+        <v>2</v>
+      </c>
+      <c r="J127">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>10</v>
+      </c>
+      <c r="B128">
+        <v>61</v>
+      </c>
+      <c r="C128" t="b">
+        <v>1</v>
+      </c>
+      <c r="D128" t="b">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0.5</v>
+      </c>
+      <c r="F128">
+        <v>0.05</v>
+      </c>
+      <c r="G128" t="s">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>1000</v>
+      </c>
+      <c r="I128">
+        <v>2</v>
+      </c>
+      <c r="J128">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129">
+        <v>62</v>
+      </c>
+      <c r="C129" t="b">
+        <v>1</v>
+      </c>
+      <c r="D129" t="b">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0.5</v>
+      </c>
+      <c r="F129">
+        <v>0.05</v>
+      </c>
+      <c r="G129" t="s">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>1000</v>
+      </c>
+      <c r="I129">
+        <v>2</v>
+      </c>
+      <c r="J129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>10</v>
+      </c>
+      <c r="B130">
+        <v>63</v>
+      </c>
+      <c r="C130" t="b">
+        <v>1</v>
+      </c>
+      <c r="D130" t="b">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0.5</v>
+      </c>
+      <c r="F130">
+        <v>0.05</v>
+      </c>
+      <c r="G130" t="s">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>1000</v>
+      </c>
+      <c r="I130">
+        <v>2</v>
+      </c>
+      <c r="J130">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>10</v>
+      </c>
+      <c r="B131">
+        <v>64</v>
+      </c>
+      <c r="C131" t="b">
+        <v>1</v>
+      </c>
+      <c r="D131" t="b">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0.5</v>
+      </c>
+      <c r="F131">
+        <v>0.05</v>
+      </c>
+      <c r="G131" t="s">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>1000</v>
+      </c>
+      <c r="I131">
+        <v>2</v>
+      </c>
+      <c r="J131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132">
+        <v>65</v>
+      </c>
+      <c r="C132" t="b">
+        <v>1</v>
+      </c>
+      <c r="D132" t="b">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>0.5</v>
+      </c>
+      <c r="F132">
+        <v>0.05</v>
+      </c>
+      <c r="G132" t="s">
+        <v>0</v>
+      </c>
+      <c r="H132">
+        <v>1000</v>
+      </c>
+      <c r="I132">
+        <v>2</v>
+      </c>
+      <c r="J132">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>10</v>
+      </c>
+      <c r="B133">
+        <v>66</v>
+      </c>
+      <c r="C133" t="b">
+        <v>1</v>
+      </c>
+      <c r="D133" t="b">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0.5</v>
+      </c>
+      <c r="F133">
+        <v>0.05</v>
+      </c>
+      <c r="G133" t="s">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>1000</v>
+      </c>
+      <c r="I133">
+        <v>2</v>
+      </c>
+      <c r="J133">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134">
+        <v>67</v>
+      </c>
+      <c r="C134" t="b">
+        <v>1</v>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>0.5</v>
+      </c>
+      <c r="F134">
+        <v>0.05</v>
+      </c>
+      <c r="G134" t="s">
+        <v>0</v>
+      </c>
+      <c r="H134">
+        <v>1000</v>
+      </c>
+      <c r="I134">
+        <v>2</v>
+      </c>
+      <c r="J134">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135">
+        <v>68</v>
+      </c>
+      <c r="C135" t="b">
+        <v>1</v>
+      </c>
+      <c r="D135" t="b">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>0.5</v>
+      </c>
+      <c r="F135">
+        <v>0.05</v>
+      </c>
+      <c r="G135" t="s">
+        <v>0</v>
+      </c>
+      <c r="H135">
+        <v>1000</v>
+      </c>
+      <c r="I135">
+        <v>2</v>
+      </c>
+      <c r="J135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136">
+        <v>69</v>
+      </c>
+      <c r="C136" t="b">
+        <v>1</v>
+      </c>
+      <c r="D136" t="b">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0.5</v>
+      </c>
+      <c r="F136">
+        <v>0.05</v>
+      </c>
+      <c r="G136" t="s">
+        <v>0</v>
+      </c>
+      <c r="H136">
+        <v>1000</v>
+      </c>
+      <c r="I136">
+        <v>2</v>
+      </c>
+      <c r="J136">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137">
+        <v>70</v>
+      </c>
+      <c r="C137" t="b">
+        <v>1</v>
+      </c>
+      <c r="D137" t="b">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0.5</v>
+      </c>
+      <c r="F137">
+        <v>0.05</v>
+      </c>
+      <c r="G137" t="s">
+        <v>0</v>
+      </c>
+      <c r="H137">
+        <v>1000</v>
+      </c>
+      <c r="I137">
+        <v>2</v>
+      </c>
+      <c r="J137">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138">
+        <v>71</v>
+      </c>
+      <c r="C138" t="b">
+        <v>1</v>
+      </c>
+      <c r="D138" t="b">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0.5</v>
+      </c>
+      <c r="F138">
+        <v>0.05</v>
+      </c>
+      <c r="G138" t="s">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>1000</v>
+      </c>
+      <c r="I138">
+        <v>2</v>
+      </c>
+      <c r="J138">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>10</v>
+      </c>
+      <c r="B139">
+        <v>72</v>
+      </c>
+      <c r="C139" t="b">
+        <v>1</v>
+      </c>
+      <c r="D139" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0.5</v>
+      </c>
+      <c r="F139">
+        <v>0.05</v>
+      </c>
+      <c r="G139" t="s">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>1000</v>
+      </c>
+      <c r="I139">
+        <v>2</v>
+      </c>
+      <c r="J139">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140">
+        <v>73</v>
+      </c>
+      <c r="C140" t="b">
+        <v>1</v>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0.5</v>
+      </c>
+      <c r="F140">
+        <v>0.05</v>
+      </c>
+      <c r="G140" t="s">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>1000</v>
+      </c>
+      <c r="I140">
+        <v>2</v>
+      </c>
+      <c r="J140">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>10</v>
+      </c>
+      <c r="B141">
+        <v>74</v>
+      </c>
+      <c r="C141" t="b">
+        <v>1</v>
+      </c>
+      <c r="D141" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0.5</v>
+      </c>
+      <c r="F141">
+        <v>0.05</v>
+      </c>
+      <c r="G141" t="s">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>1000</v>
+      </c>
+      <c r="I141">
+        <v>2</v>
+      </c>
+      <c r="J141">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>10</v>
+      </c>
+      <c r="B142">
+        <v>75</v>
+      </c>
+      <c r="C142" t="b">
+        <v>1</v>
+      </c>
+      <c r="D142" t="b">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0.5</v>
+      </c>
+      <c r="F142">
+        <v>0.05</v>
+      </c>
+      <c r="G142" t="s">
+        <v>0</v>
+      </c>
+      <c r="H142">
+        <v>1000</v>
+      </c>
+      <c r="I142">
+        <v>2</v>
+      </c>
+      <c r="J142">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>10</v>
+      </c>
+      <c r="B143">
+        <v>76</v>
+      </c>
+      <c r="C143" t="b">
+        <v>1</v>
+      </c>
+      <c r="D143" t="b">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0.5</v>
+      </c>
+      <c r="F143">
+        <v>0.05</v>
+      </c>
+      <c r="G143" t="s">
+        <v>0</v>
+      </c>
+      <c r="H143">
+        <v>1000</v>
+      </c>
+      <c r="I143">
+        <v>2</v>
+      </c>
+      <c r="J143">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>10</v>
+      </c>
+      <c r="B144">
+        <v>77</v>
+      </c>
+      <c r="C144" t="b">
+        <v>1</v>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>0.5</v>
+      </c>
+      <c r="F144">
+        <v>0.05</v>
+      </c>
+      <c r="G144" t="s">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>1000</v>
+      </c>
+      <c r="I144">
+        <v>2</v>
+      </c>
+      <c r="J144">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>10</v>
+      </c>
+      <c r="B145">
+        <v>78</v>
+      </c>
+      <c r="C145" t="b">
+        <v>1</v>
+      </c>
+      <c r="D145" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0.5</v>
+      </c>
+      <c r="F145">
+        <v>0.05</v>
+      </c>
+      <c r="G145" t="s">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>1000</v>
+      </c>
+      <c r="I145">
+        <v>2</v>
+      </c>
+      <c r="J145">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>10</v>
+      </c>
+      <c r="B146">
+        <v>79</v>
+      </c>
+      <c r="C146" t="b">
+        <v>1</v>
+      </c>
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>0.5</v>
+      </c>
+      <c r="F146">
+        <v>0.05</v>
+      </c>
+      <c r="G146" t="s">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>1000</v>
+      </c>
+      <c r="I146">
+        <v>2</v>
+      </c>
+      <c r="J146">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>10</v>
+      </c>
+      <c r="B147">
+        <v>80</v>
+      </c>
+      <c r="C147" t="b">
+        <v>1</v>
+      </c>
+      <c r="D147" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0.5</v>
+      </c>
+      <c r="F147">
+        <v>0.05</v>
+      </c>
+      <c r="G147" t="s">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>1000</v>
+      </c>
+      <c r="I147">
+        <v>2</v>
+      </c>
+      <c r="J147">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>10</v>
+      </c>
+      <c r="B148">
+        <v>81</v>
+      </c>
+      <c r="C148" t="b">
+        <v>1</v>
+      </c>
+      <c r="D148" t="b">
+        <v>0</v>
+      </c>
+      <c r="E148">
+        <v>0.5</v>
+      </c>
+      <c r="F148">
+        <v>0.05</v>
+      </c>
+      <c r="G148" t="s">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>1000</v>
+      </c>
+      <c r="I148">
+        <v>2</v>
+      </c>
+      <c r="J148">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>10</v>
+      </c>
+      <c r="B149">
+        <v>82</v>
+      </c>
+      <c r="C149" t="b">
+        <v>1</v>
+      </c>
+      <c r="D149" t="b">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0.5</v>
+      </c>
+      <c r="F149">
+        <v>0.05</v>
+      </c>
+      <c r="G149" t="s">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>1000</v>
+      </c>
+      <c r="I149">
+        <v>2</v>
+      </c>
+      <c r="J149">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>10</v>
+      </c>
+      <c r="B150">
+        <v>83</v>
+      </c>
+      <c r="C150" t="b">
+        <v>1</v>
+      </c>
+      <c r="D150" t="b">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0.5</v>
+      </c>
+      <c r="F150">
+        <v>0.05</v>
+      </c>
+      <c r="G150" t="s">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>1000</v>
+      </c>
+      <c r="I150">
+        <v>2</v>
+      </c>
+      <c r="J150">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>10</v>
+      </c>
+      <c r="B151">
+        <v>84</v>
+      </c>
+      <c r="C151" t="b">
+        <v>1</v>
+      </c>
+      <c r="D151" t="b">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0.5</v>
+      </c>
+      <c r="F151">
+        <v>0.05</v>
+      </c>
+      <c r="G151" t="s">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>1000</v>
+      </c>
+      <c r="I151">
+        <v>2</v>
+      </c>
+      <c r="J151">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>10</v>
+      </c>
+      <c r="B152">
+        <v>85</v>
+      </c>
+      <c r="C152" t="b">
+        <v>1</v>
+      </c>
+      <c r="D152" t="b">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0.5</v>
+      </c>
+      <c r="F152">
+        <v>0.05</v>
+      </c>
+      <c r="G152" t="s">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>1000</v>
+      </c>
+      <c r="I152">
+        <v>2</v>
+      </c>
+      <c r="J152">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>10</v>
+      </c>
+      <c r="B153">
+        <v>86</v>
+      </c>
+      <c r="C153" t="b">
+        <v>1</v>
+      </c>
+      <c r="D153" t="b">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0.5</v>
+      </c>
+      <c r="F153">
+        <v>0.05</v>
+      </c>
+      <c r="G153" t="s">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>1000</v>
+      </c>
+      <c r="I153">
+        <v>2</v>
+      </c>
+      <c r="J153">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>10</v>
+      </c>
+      <c r="B154">
+        <v>87</v>
+      </c>
+      <c r="C154" t="b">
+        <v>1</v>
+      </c>
+      <c r="D154" t="b">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0.5</v>
+      </c>
+      <c r="F154">
+        <v>0.05</v>
+      </c>
+      <c r="G154" t="s">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>1000</v>
+      </c>
+      <c r="I154">
+        <v>2</v>
+      </c>
+      <c r="J154">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>10</v>
+      </c>
+      <c r="B155">
+        <v>88</v>
+      </c>
+      <c r="C155" t="b">
+        <v>1</v>
+      </c>
+      <c r="D155" t="b">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>0.5</v>
+      </c>
+      <c r="F155">
+        <v>0.05</v>
+      </c>
+      <c r="G155" t="s">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>1000</v>
+      </c>
+      <c r="I155">
+        <v>2</v>
+      </c>
+      <c r="J155">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>10</v>
+      </c>
+      <c r="B156">
+        <v>89</v>
+      </c>
+      <c r="C156" t="b">
+        <v>1</v>
+      </c>
+      <c r="D156" t="b">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0.5</v>
+      </c>
+      <c r="F156">
+        <v>0.05</v>
+      </c>
+      <c r="G156" t="s">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>1000</v>
+      </c>
+      <c r="I156">
+        <v>2</v>
+      </c>
+      <c r="J156">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>10</v>
+      </c>
+      <c r="B157">
+        <v>90</v>
+      </c>
+      <c r="C157" t="b">
+        <v>1</v>
+      </c>
+      <c r="D157" t="b">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0.5</v>
+      </c>
+      <c r="F157">
+        <v>0.05</v>
+      </c>
+      <c r="G157" t="s">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>1000</v>
+      </c>
+      <c r="I157">
+        <v>2</v>
+      </c>
+      <c r="J157">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>10</v>
+      </c>
+      <c r="B158">
+        <v>91</v>
+      </c>
+      <c r="C158" t="b">
+        <v>1</v>
+      </c>
+      <c r="D158" t="b">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0.5</v>
+      </c>
+      <c r="F158">
+        <v>0.05</v>
+      </c>
+      <c r="G158" t="s">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>1000</v>
+      </c>
+      <c r="I158">
+        <v>2</v>
+      </c>
+      <c r="J158">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>10</v>
+      </c>
+      <c r="B159">
+        <v>92</v>
+      </c>
+      <c r="C159" t="b">
+        <v>1</v>
+      </c>
+      <c r="D159" t="b">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0.5</v>
+      </c>
+      <c r="F159">
+        <v>0.05</v>
+      </c>
+      <c r="G159" t="s">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>1000</v>
+      </c>
+      <c r="I159">
+        <v>2</v>
+      </c>
+      <c r="J159">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>10</v>
+      </c>
+      <c r="B160">
+        <v>93</v>
+      </c>
+      <c r="C160" t="b">
+        <v>1</v>
+      </c>
+      <c r="D160" t="b">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0.5</v>
+      </c>
+      <c r="F160">
+        <v>0.05</v>
+      </c>
+      <c r="G160" t="s">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>1000</v>
+      </c>
+      <c r="I160">
+        <v>2</v>
+      </c>
+      <c r="J160">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>10</v>
+      </c>
+      <c r="B161">
+        <v>94</v>
+      </c>
+      <c r="C161" t="b">
+        <v>1</v>
+      </c>
+      <c r="D161" t="b">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>0.5</v>
+      </c>
+      <c r="F161">
+        <v>0.05</v>
+      </c>
+      <c r="G161" t="s">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>1000</v>
+      </c>
+      <c r="I161">
+        <v>2</v>
+      </c>
+      <c r="J161">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>10</v>
+      </c>
+      <c r="B162">
+        <v>95</v>
+      </c>
+      <c r="C162" t="b">
+        <v>1</v>
+      </c>
+      <c r="D162" t="b">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0.5</v>
+      </c>
+      <c r="F162">
+        <v>0.05</v>
+      </c>
+      <c r="G162" t="s">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>1000</v>
+      </c>
+      <c r="I162">
+        <v>2</v>
+      </c>
+      <c r="J162">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>10</v>
+      </c>
+      <c r="B163">
+        <v>96</v>
+      </c>
+      <c r="C163" t="b">
+        <v>1</v>
+      </c>
+      <c r="D163" t="b">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0.5</v>
+      </c>
+      <c r="F163">
+        <v>0.05</v>
+      </c>
+      <c r="G163" t="s">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>1000</v>
+      </c>
+      <c r="I163">
+        <v>2</v>
+      </c>
+      <c r="J163">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>10</v>
+      </c>
+      <c r="B164">
+        <v>97</v>
+      </c>
+      <c r="C164" t="b">
+        <v>1</v>
+      </c>
+      <c r="D164" t="b">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>0.5</v>
+      </c>
+      <c r="F164">
+        <v>0.05</v>
+      </c>
+      <c r="G164" t="s">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>1000</v>
+      </c>
+      <c r="I164">
+        <v>2</v>
+      </c>
+      <c r="J164">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>10</v>
+      </c>
+      <c r="B165">
+        <v>98</v>
+      </c>
+      <c r="C165" t="b">
+        <v>1</v>
+      </c>
+      <c r="D165" t="b">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>0.5</v>
+      </c>
+      <c r="F165">
+        <v>0.05</v>
+      </c>
+      <c r="G165" t="s">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>1000</v>
+      </c>
+      <c r="I165">
+        <v>2</v>
+      </c>
+      <c r="J165">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166">
+        <v>99</v>
+      </c>
+      <c r="C166" t="b">
+        <v>1</v>
+      </c>
+      <c r="D166" t="b">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>0.5</v>
+      </c>
+      <c r="F166">
+        <v>0.05</v>
+      </c>
+      <c r="G166" t="s">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>1000</v>
+      </c>
+      <c r="I166">
+        <v>2</v>
+      </c>
+      <c r="J166">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>10</v>
+      </c>
+      <c r="B167">
+        <v>100</v>
+      </c>
+      <c r="C167" t="b">
+        <v>1</v>
+      </c>
+      <c r="D167" t="b">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>0.5</v>
+      </c>
+      <c r="F167">
+        <v>0.05</v>
+      </c>
+      <c r="G167" t="s">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>1000</v>
+      </c>
+      <c r="I167">
+        <v>2</v>
+      </c>
+      <c r="J167">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>10</v>
+      </c>
+      <c r="B168">
+        <v>101</v>
+      </c>
+      <c r="C168" t="b">
+        <v>1</v>
+      </c>
+      <c r="D168" t="b">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>0.5</v>
+      </c>
+      <c r="F168">
+        <v>0.05</v>
+      </c>
+      <c r="G168" t="s">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>1000</v>
+      </c>
+      <c r="I168">
+        <v>2</v>
+      </c>
+      <c r="J168">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>10</v>
+      </c>
+      <c r="B169">
+        <v>102</v>
+      </c>
+      <c r="C169" t="b">
+        <v>1</v>
+      </c>
+      <c r="D169" t="b">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>0.5</v>
+      </c>
+      <c r="F169">
+        <v>0.05</v>
+      </c>
+      <c r="G169" t="s">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>1000</v>
+      </c>
+      <c r="I169">
+        <v>2</v>
+      </c>
+      <c r="J169">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170">
+        <v>103</v>
+      </c>
+      <c r="C170" t="b">
+        <v>1</v>
+      </c>
+      <c r="D170" t="b">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>0.5</v>
+      </c>
+      <c r="F170">
+        <v>0.05</v>
+      </c>
+      <c r="G170" t="s">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>1000</v>
+      </c>
+      <c r="I170">
+        <v>2</v>
+      </c>
+      <c r="J170">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>10</v>
+      </c>
+      <c r="B171">
+        <v>104</v>
+      </c>
+      <c r="C171" t="b">
+        <v>1</v>
+      </c>
+      <c r="D171" t="b">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0.5</v>
+      </c>
+      <c r="F171">
+        <v>0.05</v>
+      </c>
+      <c r="G171" t="s">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>1000</v>
+      </c>
+      <c r="I171">
+        <v>2</v>
+      </c>
+      <c r="J171">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172">
+        <v>105</v>
+      </c>
+      <c r="C172" t="b">
+        <v>1</v>
+      </c>
+      <c r="D172" t="b">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>0.5</v>
+      </c>
+      <c r="F172">
+        <v>0.05</v>
+      </c>
+      <c r="G172" t="s">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>1000</v>
+      </c>
+      <c r="I172">
+        <v>2</v>
+      </c>
+      <c r="J172">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>10</v>
+      </c>
+      <c r="B173">
+        <v>106</v>
+      </c>
+      <c r="C173" t="b">
+        <v>1</v>
+      </c>
+      <c r="D173" t="b">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>0.5</v>
+      </c>
+      <c r="F173">
+        <v>0.05</v>
+      </c>
+      <c r="G173" t="s">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>1000</v>
+      </c>
+      <c r="I173">
+        <v>2</v>
+      </c>
+      <c r="J173">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>10</v>
+      </c>
+      <c r="B174">
+        <v>107</v>
+      </c>
+      <c r="C174" t="b">
+        <v>1</v>
+      </c>
+      <c r="D174" t="b">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0.5</v>
+      </c>
+      <c r="F174">
+        <v>0.05</v>
+      </c>
+      <c r="G174" t="s">
+        <v>0</v>
+      </c>
+      <c r="H174">
+        <v>1000</v>
+      </c>
+      <c r="I174">
+        <v>2</v>
+      </c>
+      <c r="J174">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>10</v>
+      </c>
+      <c r="B175">
+        <v>108</v>
+      </c>
+      <c r="C175" t="b">
+        <v>1</v>
+      </c>
+      <c r="D175" t="b">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>0.5</v>
+      </c>
+      <c r="F175">
+        <v>0.05</v>
+      </c>
+      <c r="G175" t="s">
+        <v>0</v>
+      </c>
+      <c r="H175">
+        <v>1000</v>
+      </c>
+      <c r="I175">
+        <v>2</v>
+      </c>
+      <c r="J175">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176">
+        <v>109</v>
+      </c>
+      <c r="C176" t="b">
+        <v>1</v>
+      </c>
+      <c r="D176" t="b">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0.5</v>
+      </c>
+      <c r="F176">
+        <v>0.05</v>
+      </c>
+      <c r="G176" t="s">
+        <v>0</v>
+      </c>
+      <c r="H176">
+        <v>1000</v>
+      </c>
+      <c r="I176">
+        <v>2</v>
+      </c>
+      <c r="J176">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>10</v>
+      </c>
+      <c r="B177">
+        <v>110</v>
+      </c>
+      <c r="C177" t="b">
+        <v>1</v>
+      </c>
+      <c r="D177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>0.5</v>
+      </c>
+      <c r="F177">
+        <v>0.05</v>
+      </c>
+      <c r="G177" t="s">
+        <v>0</v>
+      </c>
+      <c r="H177">
+        <v>1000</v>
+      </c>
+      <c r="I177">
+        <v>2</v>
+      </c>
+      <c r="J177">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>10</v>
+      </c>
+      <c r="B178">
+        <v>111</v>
+      </c>
+      <c r="C178" t="b">
+        <v>1</v>
+      </c>
+      <c r="D178" t="b">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0.5</v>
+      </c>
+      <c r="F178">
+        <v>0.05</v>
+      </c>
+      <c r="G178" t="s">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>1000</v>
+      </c>
+      <c r="I178">
+        <v>2</v>
+      </c>
+      <c r="J178">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>10</v>
+      </c>
+      <c r="B179">
+        <v>112</v>
+      </c>
+      <c r="C179" t="b">
+        <v>1</v>
+      </c>
+      <c r="D179" t="b">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0.5</v>
+      </c>
+      <c r="F179">
+        <v>0.05</v>
+      </c>
+      <c r="G179" t="s">
+        <v>0</v>
+      </c>
+      <c r="H179">
+        <v>1000</v>
+      </c>
+      <c r="I179">
+        <v>2</v>
+      </c>
+      <c r="J179">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>10</v>
+      </c>
+      <c r="B180">
+        <v>113</v>
+      </c>
+      <c r="C180" t="b">
+        <v>1</v>
+      </c>
+      <c r="D180" t="b">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0.5</v>
+      </c>
+      <c r="F180">
+        <v>0.05</v>
+      </c>
+      <c r="G180" t="s">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>1000</v>
+      </c>
+      <c r="I180">
+        <v>2</v>
+      </c>
+      <c r="J180">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>10</v>
+      </c>
+      <c r="B181">
+        <v>114</v>
+      </c>
+      <c r="C181" t="b">
+        <v>1</v>
+      </c>
+      <c r="D181" t="b">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>0.5</v>
+      </c>
+      <c r="F181">
+        <v>0.05</v>
+      </c>
+      <c r="G181" t="s">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>1000</v>
+      </c>
+      <c r="I181">
+        <v>2</v>
+      </c>
+      <c r="J181">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>10</v>
+      </c>
+      <c r="B182">
+        <v>115</v>
+      </c>
+      <c r="C182" t="b">
+        <v>1</v>
+      </c>
+      <c r="D182" t="b">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0.5</v>
+      </c>
+      <c r="F182">
+        <v>0.05</v>
+      </c>
+      <c r="G182" t="s">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>1000</v>
+      </c>
+      <c r="I182">
+        <v>2</v>
+      </c>
+      <c r="J182">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>10</v>
+      </c>
+      <c r="B183">
+        <v>116</v>
+      </c>
+      <c r="C183" t="b">
+        <v>1</v>
+      </c>
+      <c r="D183" t="b">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>0.5</v>
+      </c>
+      <c r="F183">
+        <v>0.05</v>
+      </c>
+      <c r="G183" t="s">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>1000</v>
+      </c>
+      <c r="I183">
+        <v>2</v>
+      </c>
+      <c r="J183">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>10</v>
+      </c>
+      <c r="B184">
+        <v>117</v>
+      </c>
+      <c r="C184" t="b">
+        <v>1</v>
+      </c>
+      <c r="D184" t="b">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>0.5</v>
+      </c>
+      <c r="F184">
+        <v>0.05</v>
+      </c>
+      <c r="G184" t="s">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>1000</v>
+      </c>
+      <c r="I184">
+        <v>2</v>
+      </c>
+      <c r="J184">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>10</v>
+      </c>
+      <c r="B185">
+        <v>118</v>
+      </c>
+      <c r="C185" t="b">
+        <v>1</v>
+      </c>
+      <c r="D185" t="b">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>0.5</v>
+      </c>
+      <c r="F185">
+        <v>0.05</v>
+      </c>
+      <c r="G185" t="s">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>1000</v>
+      </c>
+      <c r="I185">
+        <v>2</v>
+      </c>
+      <c r="J185">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>10</v>
+      </c>
+      <c r="B186">
+        <v>119</v>
+      </c>
+      <c r="C186" t="b">
+        <v>1</v>
+      </c>
+      <c r="D186" t="b">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>0.5</v>
+      </c>
+      <c r="F186">
+        <v>0.05</v>
+      </c>
+      <c r="G186" t="s">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>1000</v>
+      </c>
+      <c r="I186">
+        <v>2</v>
+      </c>
+      <c r="J186">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187">
+        <v>120</v>
+      </c>
+      <c r="C187" t="b">
+        <v>1</v>
+      </c>
+      <c r="D187" t="b">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>0.5</v>
+      </c>
+      <c r="F187">
+        <v>0.05</v>
+      </c>
+      <c r="G187" t="s">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>1000</v>
+      </c>
+      <c r="I187">
+        <v>2</v>
+      </c>
+      <c r="J187">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>10</v>
+      </c>
+      <c r="B188">
+        <v>121</v>
+      </c>
+      <c r="C188" t="b">
+        <v>1</v>
+      </c>
+      <c r="D188" t="b">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>0.5</v>
+      </c>
+      <c r="F188">
+        <v>0.05</v>
+      </c>
+      <c r="G188" t="s">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>1000</v>
+      </c>
+      <c r="I188">
+        <v>2</v>
+      </c>
+      <c r="J188">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>10</v>
+      </c>
+      <c r="B189">
+        <v>122</v>
+      </c>
+      <c r="C189" t="b">
+        <v>1</v>
+      </c>
+      <c r="D189" t="b">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0.5</v>
+      </c>
+      <c r="F189">
+        <v>0.05</v>
+      </c>
+      <c r="G189" t="s">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>1000</v>
+      </c>
+      <c r="I189">
+        <v>2</v>
+      </c>
+      <c r="J189">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>10</v>
+      </c>
+      <c r="B190">
+        <v>123</v>
+      </c>
+      <c r="C190" t="b">
+        <v>1</v>
+      </c>
+      <c r="D190" t="b">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>0.5</v>
+      </c>
+      <c r="F190">
+        <v>0.05</v>
+      </c>
+      <c r="G190" t="s">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>1000</v>
+      </c>
+      <c r="I190">
+        <v>2</v>
+      </c>
+      <c r="J190">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>10</v>
+      </c>
+      <c r="B191">
+        <v>124</v>
+      </c>
+      <c r="C191" t="b">
+        <v>1</v>
+      </c>
+      <c r="D191" t="b">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>0.5</v>
+      </c>
+      <c r="F191">
+        <v>0.05</v>
+      </c>
+      <c r="G191" t="s">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>1000</v>
+      </c>
+      <c r="I191">
+        <v>2</v>
+      </c>
+      <c r="J191">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>10</v>
+      </c>
+      <c r="B192">
+        <v>125</v>
+      </c>
+      <c r="C192" t="b">
+        <v>1</v>
+      </c>
+      <c r="D192" t="b">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>0.5</v>
+      </c>
+      <c r="F192">
+        <v>0.05</v>
+      </c>
+      <c r="G192" t="s">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>1000</v>
+      </c>
+      <c r="I192">
+        <v>2</v>
+      </c>
+      <c r="J192">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
No LDA mallet Completed 77
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14E1D8-8FE0-8347-8FF8-45323D877587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE925E5-A564-BF43-BC00-0DDDED9039BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="12">
   <si>
     <t>auto</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J192"/>
+  <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="L191" sqref="L191"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2919,7 +2919,7 @@
         <v>10</v>
       </c>
       <c r="B79">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="C79" t="b">
         <v>1</v>
@@ -2951,7 +2951,7 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="C80" t="b">
         <v>1</v>
@@ -2983,7 +2983,7 @@
         <v>10</v>
       </c>
       <c r="B81">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="C81" t="b">
         <v>1</v>
@@ -3015,7 +3015,7 @@
         <v>10</v>
       </c>
       <c r="B82">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="C82" t="b">
         <v>1</v>
@@ -3047,7 +3047,7 @@
         <v>10</v>
       </c>
       <c r="B83">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="C83" t="b">
         <v>1</v>
@@ -3079,7 +3079,7 @@
         <v>10</v>
       </c>
       <c r="B84">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C84" t="b">
         <v>1</v>
@@ -3111,7 +3111,7 @@
         <v>10</v>
       </c>
       <c r="B85">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="C85" t="b">
         <v>1</v>
@@ -3143,7 +3143,7 @@
         <v>10</v>
       </c>
       <c r="B86">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C86" t="b">
         <v>1</v>
@@ -3175,7 +3175,7 @@
         <v>10</v>
       </c>
       <c r="B87">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="C87" t="b">
         <v>1</v>
@@ -3207,7 +3207,7 @@
         <v>10</v>
       </c>
       <c r="B88">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="C88" t="b">
         <v>1</v>
@@ -3219,7 +3219,7 @@
         <v>0.5</v>
       </c>
       <c r="F88">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G88" t="s">
         <v>0</v>
@@ -3239,7 +3239,7 @@
         <v>10</v>
       </c>
       <c r="B89">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="C89" t="b">
         <v>1</v>
@@ -3251,7 +3251,7 @@
         <v>0.5</v>
       </c>
       <c r="F89">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G89" t="s">
         <v>0</v>
@@ -3271,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="B90">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="C90" t="b">
         <v>1</v>
@@ -3283,7 +3283,7 @@
         <v>0.5</v>
       </c>
       <c r="F90">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G90" t="s">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>10</v>
       </c>
       <c r="B91">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="C91" t="b">
         <v>1</v>
@@ -3315,7 +3315,7 @@
         <v>0.5</v>
       </c>
       <c r="F91">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G91" t="s">
         <v>0</v>
@@ -3335,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="B92">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="C92" t="b">
         <v>1</v>
@@ -3347,7 +3347,7 @@
         <v>0.5</v>
       </c>
       <c r="F92">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G92" t="s">
         <v>0</v>
@@ -3367,7 +3367,7 @@
         <v>10</v>
       </c>
       <c r="B93">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="C93" t="b">
         <v>1</v>
@@ -3379,7 +3379,7 @@
         <v>0.5</v>
       </c>
       <c r="F93">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G93" t="s">
         <v>0</v>
@@ -3399,7 +3399,7 @@
         <v>10</v>
       </c>
       <c r="B94">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C94" t="b">
         <v>1</v>
@@ -3411,7 +3411,7 @@
         <v>0.5</v>
       </c>
       <c r="F94">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G94" t="s">
         <v>0</v>
@@ -3431,7 +3431,7 @@
         <v>10</v>
       </c>
       <c r="B95">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="C95" t="b">
         <v>1</v>
@@ -3443,7 +3443,7 @@
         <v>0.5</v>
       </c>
       <c r="F95">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G95" t="s">
         <v>0</v>
@@ -3463,7 +3463,7 @@
         <v>10</v>
       </c>
       <c r="B96">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="C96" t="b">
         <v>1</v>
@@ -3475,7 +3475,7 @@
         <v>0.5</v>
       </c>
       <c r="F96">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G96" t="s">
         <v>0</v>
@@ -3495,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="B97">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="C97" t="b">
         <v>1</v>
@@ -3507,7 +3507,7 @@
         <v>0.5</v>
       </c>
       <c r="F97">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G97" t="s">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="B98">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C98" t="b">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>0.5</v>
       </c>
       <c r="F98">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G98" t="s">
         <v>0</v>
@@ -3559,7 +3559,7 @@
         <v>10</v>
       </c>
       <c r="B99">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="C99" t="b">
         <v>1</v>
@@ -3571,7 +3571,7 @@
         <v>0.5</v>
       </c>
       <c r="F99">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G99" t="s">
         <v>0</v>
@@ -3591,7 +3591,7 @@
         <v>10</v>
       </c>
       <c r="B100">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="C100" t="b">
         <v>1</v>
@@ -3603,7 +3603,7 @@
         <v>0.5</v>
       </c>
       <c r="F100">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G100" t="s">
         <v>0</v>
@@ -3623,7 +3623,7 @@
         <v>10</v>
       </c>
       <c r="B101">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="C101" t="b">
         <v>1</v>
@@ -3635,7 +3635,7 @@
         <v>0.5</v>
       </c>
       <c r="F101">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G101" t="s">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>10</v>
       </c>
       <c r="B102">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="C102" t="b">
         <v>1</v>
@@ -3667,7 +3667,7 @@
         <v>0.5</v>
       </c>
       <c r="F102">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G102" t="s">
         <v>0</v>
@@ -3687,7 +3687,7 @@
         <v>10</v>
       </c>
       <c r="B103">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="C103" t="b">
         <v>1</v>
@@ -3699,7 +3699,7 @@
         <v>0.5</v>
       </c>
       <c r="F103">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G103" t="s">
         <v>0</v>
@@ -3719,7 +3719,7 @@
         <v>10</v>
       </c>
       <c r="B104">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="C104" t="b">
         <v>1</v>
@@ -3731,7 +3731,7 @@
         <v>0.5</v>
       </c>
       <c r="F104">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G104" t="s">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="B105">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="C105" t="b">
         <v>1</v>
@@ -3763,7 +3763,7 @@
         <v>0.5</v>
       </c>
       <c r="F105">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G105" t="s">
         <v>0</v>
@@ -3783,7 +3783,7 @@
         <v>10</v>
       </c>
       <c r="B106">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C106" t="b">
         <v>1</v>
@@ -3795,7 +3795,7 @@
         <v>0.5</v>
       </c>
       <c r="F106">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G106" t="s">
         <v>0</v>
@@ -3815,7 +3815,7 @@
         <v>10</v>
       </c>
       <c r="B107">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="C107" t="b">
         <v>1</v>
@@ -3827,7 +3827,7 @@
         <v>0.5</v>
       </c>
       <c r="F107">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G107" t="s">
         <v>0</v>
@@ -3847,7 +3847,7 @@
         <v>10</v>
       </c>
       <c r="B108">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="C108" t="b">
         <v>1</v>
@@ -3859,7 +3859,7 @@
         <v>0.5</v>
       </c>
       <c r="F108">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G108" t="s">
         <v>0</v>
@@ -3879,7 +3879,7 @@
         <v>10</v>
       </c>
       <c r="B109">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="C109" t="b">
         <v>1</v>
@@ -3891,7 +3891,7 @@
         <v>0.5</v>
       </c>
       <c r="F109">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G109" t="s">
         <v>0</v>
@@ -3911,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="B110">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="C110" t="b">
         <v>1</v>
@@ -3923,7 +3923,7 @@
         <v>0.5</v>
       </c>
       <c r="F110">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G110" t="s">
         <v>0</v>
@@ -3943,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="B111">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="C111" t="b">
         <v>1</v>
@@ -3955,7 +3955,7 @@
         <v>0.5</v>
       </c>
       <c r="F111">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G111" t="s">
         <v>0</v>
@@ -3975,7 +3975,7 @@
         <v>10</v>
       </c>
       <c r="B112">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="C112" t="b">
         <v>1</v>
@@ -3987,7 +3987,7 @@
         <v>0.5</v>
       </c>
       <c r="F112">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G112" t="s">
         <v>0</v>
@@ -3999,2566 +3999,6 @@
         <v>2</v>
       </c>
       <c r="J112">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>10</v>
-      </c>
-      <c r="B113">
-        <v>121</v>
-      </c>
-      <c r="C113" t="b">
-        <v>1</v>
-      </c>
-      <c r="D113" t="b">
-        <v>0</v>
-      </c>
-      <c r="E113">
-        <v>0.5</v>
-      </c>
-      <c r="F113">
-        <v>0.1</v>
-      </c>
-      <c r="G113" t="s">
-        <v>0</v>
-      </c>
-      <c r="H113">
-        <v>1000</v>
-      </c>
-      <c r="I113">
-        <v>2</v>
-      </c>
-      <c r="J113">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>10</v>
-      </c>
-      <c r="B114">
-        <v>122</v>
-      </c>
-      <c r="C114" t="b">
-        <v>1</v>
-      </c>
-      <c r="D114" t="b">
-        <v>0</v>
-      </c>
-      <c r="E114">
-        <v>0.5</v>
-      </c>
-      <c r="F114">
-        <v>0.1</v>
-      </c>
-      <c r="G114" t="s">
-        <v>0</v>
-      </c>
-      <c r="H114">
-        <v>1000</v>
-      </c>
-      <c r="I114">
-        <v>2</v>
-      </c>
-      <c r="J114">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>10</v>
-      </c>
-      <c r="B115">
-        <v>123</v>
-      </c>
-      <c r="C115" t="b">
-        <v>1</v>
-      </c>
-      <c r="D115" t="b">
-        <v>0</v>
-      </c>
-      <c r="E115">
-        <v>0.5</v>
-      </c>
-      <c r="F115">
-        <v>0.1</v>
-      </c>
-      <c r="G115" t="s">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>1000</v>
-      </c>
-      <c r="I115">
-        <v>2</v>
-      </c>
-      <c r="J115">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>10</v>
-      </c>
-      <c r="B116">
-        <v>124</v>
-      </c>
-      <c r="C116" t="b">
-        <v>1</v>
-      </c>
-      <c r="D116" t="b">
-        <v>0</v>
-      </c>
-      <c r="E116">
-        <v>0.5</v>
-      </c>
-      <c r="F116">
-        <v>0.1</v>
-      </c>
-      <c r="G116" t="s">
-        <v>0</v>
-      </c>
-      <c r="H116">
-        <v>1000</v>
-      </c>
-      <c r="I116">
-        <v>2</v>
-      </c>
-      <c r="J116">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>10</v>
-      </c>
-      <c r="B117">
-        <v>125</v>
-      </c>
-      <c r="C117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D117" t="b">
-        <v>0</v>
-      </c>
-      <c r="E117">
-        <v>0.5</v>
-      </c>
-      <c r="F117">
-        <v>0.1</v>
-      </c>
-      <c r="G117" t="s">
-        <v>0</v>
-      </c>
-      <c r="H117">
-        <v>1000</v>
-      </c>
-      <c r="I117">
-        <v>2</v>
-      </c>
-      <c r="J117">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>10</v>
-      </c>
-      <c r="B118">
-        <v>51</v>
-      </c>
-      <c r="C118" t="b">
-        <v>1</v>
-      </c>
-      <c r="D118" t="b">
-        <v>0</v>
-      </c>
-      <c r="E118">
-        <v>0.5</v>
-      </c>
-      <c r="F118">
-        <v>0.05</v>
-      </c>
-      <c r="G118" t="s">
-        <v>0</v>
-      </c>
-      <c r="H118">
-        <v>1000</v>
-      </c>
-      <c r="I118">
-        <v>2</v>
-      </c>
-      <c r="J118">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>10</v>
-      </c>
-      <c r="B119">
-        <v>52</v>
-      </c>
-      <c r="C119" t="b">
-        <v>1</v>
-      </c>
-      <c r="D119" t="b">
-        <v>0</v>
-      </c>
-      <c r="E119">
-        <v>0.5</v>
-      </c>
-      <c r="F119">
-        <v>0.05</v>
-      </c>
-      <c r="G119" t="s">
-        <v>0</v>
-      </c>
-      <c r="H119">
-        <v>1000</v>
-      </c>
-      <c r="I119">
-        <v>2</v>
-      </c>
-      <c r="J119">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>10</v>
-      </c>
-      <c r="B120">
-        <v>53</v>
-      </c>
-      <c r="C120" t="b">
-        <v>1</v>
-      </c>
-      <c r="D120" t="b">
-        <v>0</v>
-      </c>
-      <c r="E120">
-        <v>0.5</v>
-      </c>
-      <c r="F120">
-        <v>0.05</v>
-      </c>
-      <c r="G120" t="s">
-        <v>0</v>
-      </c>
-      <c r="H120">
-        <v>1000</v>
-      </c>
-      <c r="I120">
-        <v>2</v>
-      </c>
-      <c r="J120">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>10</v>
-      </c>
-      <c r="B121">
-        <v>54</v>
-      </c>
-      <c r="C121" t="b">
-        <v>1</v>
-      </c>
-      <c r="D121" t="b">
-        <v>0</v>
-      </c>
-      <c r="E121">
-        <v>0.5</v>
-      </c>
-      <c r="F121">
-        <v>0.05</v>
-      </c>
-      <c r="G121" t="s">
-        <v>0</v>
-      </c>
-      <c r="H121">
-        <v>1000</v>
-      </c>
-      <c r="I121">
-        <v>2</v>
-      </c>
-      <c r="J121">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>10</v>
-      </c>
-      <c r="B122">
-        <v>55</v>
-      </c>
-      <c r="C122" t="b">
-        <v>1</v>
-      </c>
-      <c r="D122" t="b">
-        <v>0</v>
-      </c>
-      <c r="E122">
-        <v>0.5</v>
-      </c>
-      <c r="F122">
-        <v>0.05</v>
-      </c>
-      <c r="G122" t="s">
-        <v>0</v>
-      </c>
-      <c r="H122">
-        <v>1000</v>
-      </c>
-      <c r="I122">
-        <v>2</v>
-      </c>
-      <c r="J122">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>10</v>
-      </c>
-      <c r="B123">
-        <v>56</v>
-      </c>
-      <c r="C123" t="b">
-        <v>1</v>
-      </c>
-      <c r="D123" t="b">
-        <v>0</v>
-      </c>
-      <c r="E123">
-        <v>0.5</v>
-      </c>
-      <c r="F123">
-        <v>0.05</v>
-      </c>
-      <c r="G123" t="s">
-        <v>0</v>
-      </c>
-      <c r="H123">
-        <v>1000</v>
-      </c>
-      <c r="I123">
-        <v>2</v>
-      </c>
-      <c r="J123">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>10</v>
-      </c>
-      <c r="B124">
-        <v>57</v>
-      </c>
-      <c r="C124" t="b">
-        <v>1</v>
-      </c>
-      <c r="D124" t="b">
-        <v>0</v>
-      </c>
-      <c r="E124">
-        <v>0.5</v>
-      </c>
-      <c r="F124">
-        <v>0.05</v>
-      </c>
-      <c r="G124" t="s">
-        <v>0</v>
-      </c>
-      <c r="H124">
-        <v>1000</v>
-      </c>
-      <c r="I124">
-        <v>2</v>
-      </c>
-      <c r="J124">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>10</v>
-      </c>
-      <c r="B125">
-        <v>58</v>
-      </c>
-      <c r="C125" t="b">
-        <v>1</v>
-      </c>
-      <c r="D125" t="b">
-        <v>0</v>
-      </c>
-      <c r="E125">
-        <v>0.5</v>
-      </c>
-      <c r="F125">
-        <v>0.05</v>
-      </c>
-      <c r="G125" t="s">
-        <v>0</v>
-      </c>
-      <c r="H125">
-        <v>1000</v>
-      </c>
-      <c r="I125">
-        <v>2</v>
-      </c>
-      <c r="J125">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>10</v>
-      </c>
-      <c r="B126">
-        <v>59</v>
-      </c>
-      <c r="C126" t="b">
-        <v>1</v>
-      </c>
-      <c r="D126" t="b">
-        <v>0</v>
-      </c>
-      <c r="E126">
-        <v>0.5</v>
-      </c>
-      <c r="F126">
-        <v>0.05</v>
-      </c>
-      <c r="G126" t="s">
-        <v>0</v>
-      </c>
-      <c r="H126">
-        <v>1000</v>
-      </c>
-      <c r="I126">
-        <v>2</v>
-      </c>
-      <c r="J126">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>10</v>
-      </c>
-      <c r="B127">
-        <v>60</v>
-      </c>
-      <c r="C127" t="b">
-        <v>1</v>
-      </c>
-      <c r="D127" t="b">
-        <v>0</v>
-      </c>
-      <c r="E127">
-        <v>0.5</v>
-      </c>
-      <c r="F127">
-        <v>0.05</v>
-      </c>
-      <c r="G127" t="s">
-        <v>0</v>
-      </c>
-      <c r="H127">
-        <v>1000</v>
-      </c>
-      <c r="I127">
-        <v>2</v>
-      </c>
-      <c r="J127">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>10</v>
-      </c>
-      <c r="B128">
-        <v>61</v>
-      </c>
-      <c r="C128" t="b">
-        <v>1</v>
-      </c>
-      <c r="D128" t="b">
-        <v>0</v>
-      </c>
-      <c r="E128">
-        <v>0.5</v>
-      </c>
-      <c r="F128">
-        <v>0.05</v>
-      </c>
-      <c r="G128" t="s">
-        <v>0</v>
-      </c>
-      <c r="H128">
-        <v>1000</v>
-      </c>
-      <c r="I128">
-        <v>2</v>
-      </c>
-      <c r="J128">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>10</v>
-      </c>
-      <c r="B129">
-        <v>62</v>
-      </c>
-      <c r="C129" t="b">
-        <v>1</v>
-      </c>
-      <c r="D129" t="b">
-        <v>0</v>
-      </c>
-      <c r="E129">
-        <v>0.5</v>
-      </c>
-      <c r="F129">
-        <v>0.05</v>
-      </c>
-      <c r="G129" t="s">
-        <v>0</v>
-      </c>
-      <c r="H129">
-        <v>1000</v>
-      </c>
-      <c r="I129">
-        <v>2</v>
-      </c>
-      <c r="J129">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>10</v>
-      </c>
-      <c r="B130">
-        <v>63</v>
-      </c>
-      <c r="C130" t="b">
-        <v>1</v>
-      </c>
-      <c r="D130" t="b">
-        <v>0</v>
-      </c>
-      <c r="E130">
-        <v>0.5</v>
-      </c>
-      <c r="F130">
-        <v>0.05</v>
-      </c>
-      <c r="G130" t="s">
-        <v>0</v>
-      </c>
-      <c r="H130">
-        <v>1000</v>
-      </c>
-      <c r="I130">
-        <v>2</v>
-      </c>
-      <c r="J130">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>10</v>
-      </c>
-      <c r="B131">
-        <v>64</v>
-      </c>
-      <c r="C131" t="b">
-        <v>1</v>
-      </c>
-      <c r="D131" t="b">
-        <v>0</v>
-      </c>
-      <c r="E131">
-        <v>0.5</v>
-      </c>
-      <c r="F131">
-        <v>0.05</v>
-      </c>
-      <c r="G131" t="s">
-        <v>0</v>
-      </c>
-      <c r="H131">
-        <v>1000</v>
-      </c>
-      <c r="I131">
-        <v>2</v>
-      </c>
-      <c r="J131">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>10</v>
-      </c>
-      <c r="B132">
-        <v>65</v>
-      </c>
-      <c r="C132" t="b">
-        <v>1</v>
-      </c>
-      <c r="D132" t="b">
-        <v>0</v>
-      </c>
-      <c r="E132">
-        <v>0.5</v>
-      </c>
-      <c r="F132">
-        <v>0.05</v>
-      </c>
-      <c r="G132" t="s">
-        <v>0</v>
-      </c>
-      <c r="H132">
-        <v>1000</v>
-      </c>
-      <c r="I132">
-        <v>2</v>
-      </c>
-      <c r="J132">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>10</v>
-      </c>
-      <c r="B133">
-        <v>66</v>
-      </c>
-      <c r="C133" t="b">
-        <v>1</v>
-      </c>
-      <c r="D133" t="b">
-        <v>0</v>
-      </c>
-      <c r="E133">
-        <v>0.5</v>
-      </c>
-      <c r="F133">
-        <v>0.05</v>
-      </c>
-      <c r="G133" t="s">
-        <v>0</v>
-      </c>
-      <c r="H133">
-        <v>1000</v>
-      </c>
-      <c r="I133">
-        <v>2</v>
-      </c>
-      <c r="J133">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>10</v>
-      </c>
-      <c r="B134">
-        <v>67</v>
-      </c>
-      <c r="C134" t="b">
-        <v>1</v>
-      </c>
-      <c r="D134" t="b">
-        <v>0</v>
-      </c>
-      <c r="E134">
-        <v>0.5</v>
-      </c>
-      <c r="F134">
-        <v>0.05</v>
-      </c>
-      <c r="G134" t="s">
-        <v>0</v>
-      </c>
-      <c r="H134">
-        <v>1000</v>
-      </c>
-      <c r="I134">
-        <v>2</v>
-      </c>
-      <c r="J134">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>10</v>
-      </c>
-      <c r="B135">
-        <v>68</v>
-      </c>
-      <c r="C135" t="b">
-        <v>1</v>
-      </c>
-      <c r="D135" t="b">
-        <v>0</v>
-      </c>
-      <c r="E135">
-        <v>0.5</v>
-      </c>
-      <c r="F135">
-        <v>0.05</v>
-      </c>
-      <c r="G135" t="s">
-        <v>0</v>
-      </c>
-      <c r="H135">
-        <v>1000</v>
-      </c>
-      <c r="I135">
-        <v>2</v>
-      </c>
-      <c r="J135">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>10</v>
-      </c>
-      <c r="B136">
-        <v>69</v>
-      </c>
-      <c r="C136" t="b">
-        <v>1</v>
-      </c>
-      <c r="D136" t="b">
-        <v>0</v>
-      </c>
-      <c r="E136">
-        <v>0.5</v>
-      </c>
-      <c r="F136">
-        <v>0.05</v>
-      </c>
-      <c r="G136" t="s">
-        <v>0</v>
-      </c>
-      <c r="H136">
-        <v>1000</v>
-      </c>
-      <c r="I136">
-        <v>2</v>
-      </c>
-      <c r="J136">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>10</v>
-      </c>
-      <c r="B137">
-        <v>70</v>
-      </c>
-      <c r="C137" t="b">
-        <v>1</v>
-      </c>
-      <c r="D137" t="b">
-        <v>0</v>
-      </c>
-      <c r="E137">
-        <v>0.5</v>
-      </c>
-      <c r="F137">
-        <v>0.05</v>
-      </c>
-      <c r="G137" t="s">
-        <v>0</v>
-      </c>
-      <c r="H137">
-        <v>1000</v>
-      </c>
-      <c r="I137">
-        <v>2</v>
-      </c>
-      <c r="J137">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>10</v>
-      </c>
-      <c r="B138">
-        <v>71</v>
-      </c>
-      <c r="C138" t="b">
-        <v>1</v>
-      </c>
-      <c r="D138" t="b">
-        <v>0</v>
-      </c>
-      <c r="E138">
-        <v>0.5</v>
-      </c>
-      <c r="F138">
-        <v>0.05</v>
-      </c>
-      <c r="G138" t="s">
-        <v>0</v>
-      </c>
-      <c r="H138">
-        <v>1000</v>
-      </c>
-      <c r="I138">
-        <v>2</v>
-      </c>
-      <c r="J138">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>10</v>
-      </c>
-      <c r="B139">
-        <v>72</v>
-      </c>
-      <c r="C139" t="b">
-        <v>1</v>
-      </c>
-      <c r="D139" t="b">
-        <v>0</v>
-      </c>
-      <c r="E139">
-        <v>0.5</v>
-      </c>
-      <c r="F139">
-        <v>0.05</v>
-      </c>
-      <c r="G139" t="s">
-        <v>0</v>
-      </c>
-      <c r="H139">
-        <v>1000</v>
-      </c>
-      <c r="I139">
-        <v>2</v>
-      </c>
-      <c r="J139">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>10</v>
-      </c>
-      <c r="B140">
-        <v>73</v>
-      </c>
-      <c r="C140" t="b">
-        <v>1</v>
-      </c>
-      <c r="D140" t="b">
-        <v>0</v>
-      </c>
-      <c r="E140">
-        <v>0.5</v>
-      </c>
-      <c r="F140">
-        <v>0.05</v>
-      </c>
-      <c r="G140" t="s">
-        <v>0</v>
-      </c>
-      <c r="H140">
-        <v>1000</v>
-      </c>
-      <c r="I140">
-        <v>2</v>
-      </c>
-      <c r="J140">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>10</v>
-      </c>
-      <c r="B141">
-        <v>74</v>
-      </c>
-      <c r="C141" t="b">
-        <v>1</v>
-      </c>
-      <c r="D141" t="b">
-        <v>0</v>
-      </c>
-      <c r="E141">
-        <v>0.5</v>
-      </c>
-      <c r="F141">
-        <v>0.05</v>
-      </c>
-      <c r="G141" t="s">
-        <v>0</v>
-      </c>
-      <c r="H141">
-        <v>1000</v>
-      </c>
-      <c r="I141">
-        <v>2</v>
-      </c>
-      <c r="J141">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>10</v>
-      </c>
-      <c r="B142">
-        <v>75</v>
-      </c>
-      <c r="C142" t="b">
-        <v>1</v>
-      </c>
-      <c r="D142" t="b">
-        <v>0</v>
-      </c>
-      <c r="E142">
-        <v>0.5</v>
-      </c>
-      <c r="F142">
-        <v>0.05</v>
-      </c>
-      <c r="G142" t="s">
-        <v>0</v>
-      </c>
-      <c r="H142">
-        <v>1000</v>
-      </c>
-      <c r="I142">
-        <v>2</v>
-      </c>
-      <c r="J142">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>10</v>
-      </c>
-      <c r="B143">
-        <v>76</v>
-      </c>
-      <c r="C143" t="b">
-        <v>1</v>
-      </c>
-      <c r="D143" t="b">
-        <v>0</v>
-      </c>
-      <c r="E143">
-        <v>0.5</v>
-      </c>
-      <c r="F143">
-        <v>0.05</v>
-      </c>
-      <c r="G143" t="s">
-        <v>0</v>
-      </c>
-      <c r="H143">
-        <v>1000</v>
-      </c>
-      <c r="I143">
-        <v>2</v>
-      </c>
-      <c r="J143">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>10</v>
-      </c>
-      <c r="B144">
-        <v>77</v>
-      </c>
-      <c r="C144" t="b">
-        <v>1</v>
-      </c>
-      <c r="D144" t="b">
-        <v>0</v>
-      </c>
-      <c r="E144">
-        <v>0.5</v>
-      </c>
-      <c r="F144">
-        <v>0.05</v>
-      </c>
-      <c r="G144" t="s">
-        <v>0</v>
-      </c>
-      <c r="H144">
-        <v>1000</v>
-      </c>
-      <c r="I144">
-        <v>2</v>
-      </c>
-      <c r="J144">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>10</v>
-      </c>
-      <c r="B145">
-        <v>78</v>
-      </c>
-      <c r="C145" t="b">
-        <v>1</v>
-      </c>
-      <c r="D145" t="b">
-        <v>0</v>
-      </c>
-      <c r="E145">
-        <v>0.5</v>
-      </c>
-      <c r="F145">
-        <v>0.05</v>
-      </c>
-      <c r="G145" t="s">
-        <v>0</v>
-      </c>
-      <c r="H145">
-        <v>1000</v>
-      </c>
-      <c r="I145">
-        <v>2</v>
-      </c>
-      <c r="J145">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>10</v>
-      </c>
-      <c r="B146">
-        <v>79</v>
-      </c>
-      <c r="C146" t="b">
-        <v>1</v>
-      </c>
-      <c r="D146" t="b">
-        <v>0</v>
-      </c>
-      <c r="E146">
-        <v>0.5</v>
-      </c>
-      <c r="F146">
-        <v>0.05</v>
-      </c>
-      <c r="G146" t="s">
-        <v>0</v>
-      </c>
-      <c r="H146">
-        <v>1000</v>
-      </c>
-      <c r="I146">
-        <v>2</v>
-      </c>
-      <c r="J146">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>10</v>
-      </c>
-      <c r="B147">
-        <v>80</v>
-      </c>
-      <c r="C147" t="b">
-        <v>1</v>
-      </c>
-      <c r="D147" t="b">
-        <v>0</v>
-      </c>
-      <c r="E147">
-        <v>0.5</v>
-      </c>
-      <c r="F147">
-        <v>0.05</v>
-      </c>
-      <c r="G147" t="s">
-        <v>0</v>
-      </c>
-      <c r="H147">
-        <v>1000</v>
-      </c>
-      <c r="I147">
-        <v>2</v>
-      </c>
-      <c r="J147">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>10</v>
-      </c>
-      <c r="B148">
-        <v>81</v>
-      </c>
-      <c r="C148" t="b">
-        <v>1</v>
-      </c>
-      <c r="D148" t="b">
-        <v>0</v>
-      </c>
-      <c r="E148">
-        <v>0.5</v>
-      </c>
-      <c r="F148">
-        <v>0.05</v>
-      </c>
-      <c r="G148" t="s">
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <v>1000</v>
-      </c>
-      <c r="I148">
-        <v>2</v>
-      </c>
-      <c r="J148">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>10</v>
-      </c>
-      <c r="B149">
-        <v>82</v>
-      </c>
-      <c r="C149" t="b">
-        <v>1</v>
-      </c>
-      <c r="D149" t="b">
-        <v>0</v>
-      </c>
-      <c r="E149">
-        <v>0.5</v>
-      </c>
-      <c r="F149">
-        <v>0.05</v>
-      </c>
-      <c r="G149" t="s">
-        <v>0</v>
-      </c>
-      <c r="H149">
-        <v>1000</v>
-      </c>
-      <c r="I149">
-        <v>2</v>
-      </c>
-      <c r="J149">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>10</v>
-      </c>
-      <c r="B150">
-        <v>83</v>
-      </c>
-      <c r="C150" t="b">
-        <v>1</v>
-      </c>
-      <c r="D150" t="b">
-        <v>0</v>
-      </c>
-      <c r="E150">
-        <v>0.5</v>
-      </c>
-      <c r="F150">
-        <v>0.05</v>
-      </c>
-      <c r="G150" t="s">
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <v>1000</v>
-      </c>
-      <c r="I150">
-        <v>2</v>
-      </c>
-      <c r="J150">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>10</v>
-      </c>
-      <c r="B151">
-        <v>84</v>
-      </c>
-      <c r="C151" t="b">
-        <v>1</v>
-      </c>
-      <c r="D151" t="b">
-        <v>0</v>
-      </c>
-      <c r="E151">
-        <v>0.5</v>
-      </c>
-      <c r="F151">
-        <v>0.05</v>
-      </c>
-      <c r="G151" t="s">
-        <v>0</v>
-      </c>
-      <c r="H151">
-        <v>1000</v>
-      </c>
-      <c r="I151">
-        <v>2</v>
-      </c>
-      <c r="J151">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>10</v>
-      </c>
-      <c r="B152">
-        <v>85</v>
-      </c>
-      <c r="C152" t="b">
-        <v>1</v>
-      </c>
-      <c r="D152" t="b">
-        <v>0</v>
-      </c>
-      <c r="E152">
-        <v>0.5</v>
-      </c>
-      <c r="F152">
-        <v>0.05</v>
-      </c>
-      <c r="G152" t="s">
-        <v>0</v>
-      </c>
-      <c r="H152">
-        <v>1000</v>
-      </c>
-      <c r="I152">
-        <v>2</v>
-      </c>
-      <c r="J152">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>10</v>
-      </c>
-      <c r="B153">
-        <v>86</v>
-      </c>
-      <c r="C153" t="b">
-        <v>1</v>
-      </c>
-      <c r="D153" t="b">
-        <v>0</v>
-      </c>
-      <c r="E153">
-        <v>0.5</v>
-      </c>
-      <c r="F153">
-        <v>0.05</v>
-      </c>
-      <c r="G153" t="s">
-        <v>0</v>
-      </c>
-      <c r="H153">
-        <v>1000</v>
-      </c>
-      <c r="I153">
-        <v>2</v>
-      </c>
-      <c r="J153">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>10</v>
-      </c>
-      <c r="B154">
-        <v>87</v>
-      </c>
-      <c r="C154" t="b">
-        <v>1</v>
-      </c>
-      <c r="D154" t="b">
-        <v>0</v>
-      </c>
-      <c r="E154">
-        <v>0.5</v>
-      </c>
-      <c r="F154">
-        <v>0.05</v>
-      </c>
-      <c r="G154" t="s">
-        <v>0</v>
-      </c>
-      <c r="H154">
-        <v>1000</v>
-      </c>
-      <c r="I154">
-        <v>2</v>
-      </c>
-      <c r="J154">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>10</v>
-      </c>
-      <c r="B155">
-        <v>88</v>
-      </c>
-      <c r="C155" t="b">
-        <v>1</v>
-      </c>
-      <c r="D155" t="b">
-        <v>0</v>
-      </c>
-      <c r="E155">
-        <v>0.5</v>
-      </c>
-      <c r="F155">
-        <v>0.05</v>
-      </c>
-      <c r="G155" t="s">
-        <v>0</v>
-      </c>
-      <c r="H155">
-        <v>1000</v>
-      </c>
-      <c r="I155">
-        <v>2</v>
-      </c>
-      <c r="J155">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>10</v>
-      </c>
-      <c r="B156">
-        <v>89</v>
-      </c>
-      <c r="C156" t="b">
-        <v>1</v>
-      </c>
-      <c r="D156" t="b">
-        <v>0</v>
-      </c>
-      <c r="E156">
-        <v>0.5</v>
-      </c>
-      <c r="F156">
-        <v>0.05</v>
-      </c>
-      <c r="G156" t="s">
-        <v>0</v>
-      </c>
-      <c r="H156">
-        <v>1000</v>
-      </c>
-      <c r="I156">
-        <v>2</v>
-      </c>
-      <c r="J156">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>10</v>
-      </c>
-      <c r="B157">
-        <v>90</v>
-      </c>
-      <c r="C157" t="b">
-        <v>1</v>
-      </c>
-      <c r="D157" t="b">
-        <v>0</v>
-      </c>
-      <c r="E157">
-        <v>0.5</v>
-      </c>
-      <c r="F157">
-        <v>0.05</v>
-      </c>
-      <c r="G157" t="s">
-        <v>0</v>
-      </c>
-      <c r="H157">
-        <v>1000</v>
-      </c>
-      <c r="I157">
-        <v>2</v>
-      </c>
-      <c r="J157">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>10</v>
-      </c>
-      <c r="B158">
-        <v>91</v>
-      </c>
-      <c r="C158" t="b">
-        <v>1</v>
-      </c>
-      <c r="D158" t="b">
-        <v>0</v>
-      </c>
-      <c r="E158">
-        <v>0.5</v>
-      </c>
-      <c r="F158">
-        <v>0.05</v>
-      </c>
-      <c r="G158" t="s">
-        <v>0</v>
-      </c>
-      <c r="H158">
-        <v>1000</v>
-      </c>
-      <c r="I158">
-        <v>2</v>
-      </c>
-      <c r="J158">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>10</v>
-      </c>
-      <c r="B159">
-        <v>92</v>
-      </c>
-      <c r="C159" t="b">
-        <v>1</v>
-      </c>
-      <c r="D159" t="b">
-        <v>0</v>
-      </c>
-      <c r="E159">
-        <v>0.5</v>
-      </c>
-      <c r="F159">
-        <v>0.05</v>
-      </c>
-      <c r="G159" t="s">
-        <v>0</v>
-      </c>
-      <c r="H159">
-        <v>1000</v>
-      </c>
-      <c r="I159">
-        <v>2</v>
-      </c>
-      <c r="J159">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>10</v>
-      </c>
-      <c r="B160">
-        <v>93</v>
-      </c>
-      <c r="C160" t="b">
-        <v>1</v>
-      </c>
-      <c r="D160" t="b">
-        <v>0</v>
-      </c>
-      <c r="E160">
-        <v>0.5</v>
-      </c>
-      <c r="F160">
-        <v>0.05</v>
-      </c>
-      <c r="G160" t="s">
-        <v>0</v>
-      </c>
-      <c r="H160">
-        <v>1000</v>
-      </c>
-      <c r="I160">
-        <v>2</v>
-      </c>
-      <c r="J160">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>10</v>
-      </c>
-      <c r="B161">
-        <v>94</v>
-      </c>
-      <c r="C161" t="b">
-        <v>1</v>
-      </c>
-      <c r="D161" t="b">
-        <v>0</v>
-      </c>
-      <c r="E161">
-        <v>0.5</v>
-      </c>
-      <c r="F161">
-        <v>0.05</v>
-      </c>
-      <c r="G161" t="s">
-        <v>0</v>
-      </c>
-      <c r="H161">
-        <v>1000</v>
-      </c>
-      <c r="I161">
-        <v>2</v>
-      </c>
-      <c r="J161">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>10</v>
-      </c>
-      <c r="B162">
-        <v>95</v>
-      </c>
-      <c r="C162" t="b">
-        <v>1</v>
-      </c>
-      <c r="D162" t="b">
-        <v>0</v>
-      </c>
-      <c r="E162">
-        <v>0.5</v>
-      </c>
-      <c r="F162">
-        <v>0.05</v>
-      </c>
-      <c r="G162" t="s">
-        <v>0</v>
-      </c>
-      <c r="H162">
-        <v>1000</v>
-      </c>
-      <c r="I162">
-        <v>2</v>
-      </c>
-      <c r="J162">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>10</v>
-      </c>
-      <c r="B163">
-        <v>96</v>
-      </c>
-      <c r="C163" t="b">
-        <v>1</v>
-      </c>
-      <c r="D163" t="b">
-        <v>0</v>
-      </c>
-      <c r="E163">
-        <v>0.5</v>
-      </c>
-      <c r="F163">
-        <v>0.05</v>
-      </c>
-      <c r="G163" t="s">
-        <v>0</v>
-      </c>
-      <c r="H163">
-        <v>1000</v>
-      </c>
-      <c r="I163">
-        <v>2</v>
-      </c>
-      <c r="J163">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>10</v>
-      </c>
-      <c r="B164">
-        <v>97</v>
-      </c>
-      <c r="C164" t="b">
-        <v>1</v>
-      </c>
-      <c r="D164" t="b">
-        <v>0</v>
-      </c>
-      <c r="E164">
-        <v>0.5</v>
-      </c>
-      <c r="F164">
-        <v>0.05</v>
-      </c>
-      <c r="G164" t="s">
-        <v>0</v>
-      </c>
-      <c r="H164">
-        <v>1000</v>
-      </c>
-      <c r="I164">
-        <v>2</v>
-      </c>
-      <c r="J164">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>10</v>
-      </c>
-      <c r="B165">
-        <v>98</v>
-      </c>
-      <c r="C165" t="b">
-        <v>1</v>
-      </c>
-      <c r="D165" t="b">
-        <v>0</v>
-      </c>
-      <c r="E165">
-        <v>0.5</v>
-      </c>
-      <c r="F165">
-        <v>0.05</v>
-      </c>
-      <c r="G165" t="s">
-        <v>0</v>
-      </c>
-      <c r="H165">
-        <v>1000</v>
-      </c>
-      <c r="I165">
-        <v>2</v>
-      </c>
-      <c r="J165">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>10</v>
-      </c>
-      <c r="B166">
-        <v>99</v>
-      </c>
-      <c r="C166" t="b">
-        <v>1</v>
-      </c>
-      <c r="D166" t="b">
-        <v>0</v>
-      </c>
-      <c r="E166">
-        <v>0.5</v>
-      </c>
-      <c r="F166">
-        <v>0.05</v>
-      </c>
-      <c r="G166" t="s">
-        <v>0</v>
-      </c>
-      <c r="H166">
-        <v>1000</v>
-      </c>
-      <c r="I166">
-        <v>2</v>
-      </c>
-      <c r="J166">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>10</v>
-      </c>
-      <c r="B167">
-        <v>100</v>
-      </c>
-      <c r="C167" t="b">
-        <v>1</v>
-      </c>
-      <c r="D167" t="b">
-        <v>0</v>
-      </c>
-      <c r="E167">
-        <v>0.5</v>
-      </c>
-      <c r="F167">
-        <v>0.05</v>
-      </c>
-      <c r="G167" t="s">
-        <v>0</v>
-      </c>
-      <c r="H167">
-        <v>1000</v>
-      </c>
-      <c r="I167">
-        <v>2</v>
-      </c>
-      <c r="J167">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>10</v>
-      </c>
-      <c r="B168">
-        <v>101</v>
-      </c>
-      <c r="C168" t="b">
-        <v>1</v>
-      </c>
-      <c r="D168" t="b">
-        <v>0</v>
-      </c>
-      <c r="E168">
-        <v>0.5</v>
-      </c>
-      <c r="F168">
-        <v>0.05</v>
-      </c>
-      <c r="G168" t="s">
-        <v>0</v>
-      </c>
-      <c r="H168">
-        <v>1000</v>
-      </c>
-      <c r="I168">
-        <v>2</v>
-      </c>
-      <c r="J168">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>10</v>
-      </c>
-      <c r="B169">
-        <v>102</v>
-      </c>
-      <c r="C169" t="b">
-        <v>1</v>
-      </c>
-      <c r="D169" t="b">
-        <v>0</v>
-      </c>
-      <c r="E169">
-        <v>0.5</v>
-      </c>
-      <c r="F169">
-        <v>0.05</v>
-      </c>
-      <c r="G169" t="s">
-        <v>0</v>
-      </c>
-      <c r="H169">
-        <v>1000</v>
-      </c>
-      <c r="I169">
-        <v>2</v>
-      </c>
-      <c r="J169">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>10</v>
-      </c>
-      <c r="B170">
-        <v>103</v>
-      </c>
-      <c r="C170" t="b">
-        <v>1</v>
-      </c>
-      <c r="D170" t="b">
-        <v>0</v>
-      </c>
-      <c r="E170">
-        <v>0.5</v>
-      </c>
-      <c r="F170">
-        <v>0.05</v>
-      </c>
-      <c r="G170" t="s">
-        <v>0</v>
-      </c>
-      <c r="H170">
-        <v>1000</v>
-      </c>
-      <c r="I170">
-        <v>2</v>
-      </c>
-      <c r="J170">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>10</v>
-      </c>
-      <c r="B171">
-        <v>104</v>
-      </c>
-      <c r="C171" t="b">
-        <v>1</v>
-      </c>
-      <c r="D171" t="b">
-        <v>0</v>
-      </c>
-      <c r="E171">
-        <v>0.5</v>
-      </c>
-      <c r="F171">
-        <v>0.05</v>
-      </c>
-      <c r="G171" t="s">
-        <v>0</v>
-      </c>
-      <c r="H171">
-        <v>1000</v>
-      </c>
-      <c r="I171">
-        <v>2</v>
-      </c>
-      <c r="J171">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>10</v>
-      </c>
-      <c r="B172">
-        <v>105</v>
-      </c>
-      <c r="C172" t="b">
-        <v>1</v>
-      </c>
-      <c r="D172" t="b">
-        <v>0</v>
-      </c>
-      <c r="E172">
-        <v>0.5</v>
-      </c>
-      <c r="F172">
-        <v>0.05</v>
-      </c>
-      <c r="G172" t="s">
-        <v>0</v>
-      </c>
-      <c r="H172">
-        <v>1000</v>
-      </c>
-      <c r="I172">
-        <v>2</v>
-      </c>
-      <c r="J172">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>10</v>
-      </c>
-      <c r="B173">
-        <v>106</v>
-      </c>
-      <c r="C173" t="b">
-        <v>1</v>
-      </c>
-      <c r="D173" t="b">
-        <v>0</v>
-      </c>
-      <c r="E173">
-        <v>0.5</v>
-      </c>
-      <c r="F173">
-        <v>0.05</v>
-      </c>
-      <c r="G173" t="s">
-        <v>0</v>
-      </c>
-      <c r="H173">
-        <v>1000</v>
-      </c>
-      <c r="I173">
-        <v>2</v>
-      </c>
-      <c r="J173">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>10</v>
-      </c>
-      <c r="B174">
-        <v>107</v>
-      </c>
-      <c r="C174" t="b">
-        <v>1</v>
-      </c>
-      <c r="D174" t="b">
-        <v>0</v>
-      </c>
-      <c r="E174">
-        <v>0.5</v>
-      </c>
-      <c r="F174">
-        <v>0.05</v>
-      </c>
-      <c r="G174" t="s">
-        <v>0</v>
-      </c>
-      <c r="H174">
-        <v>1000</v>
-      </c>
-      <c r="I174">
-        <v>2</v>
-      </c>
-      <c r="J174">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>10</v>
-      </c>
-      <c r="B175">
-        <v>108</v>
-      </c>
-      <c r="C175" t="b">
-        <v>1</v>
-      </c>
-      <c r="D175" t="b">
-        <v>0</v>
-      </c>
-      <c r="E175">
-        <v>0.5</v>
-      </c>
-      <c r="F175">
-        <v>0.05</v>
-      </c>
-      <c r="G175" t="s">
-        <v>0</v>
-      </c>
-      <c r="H175">
-        <v>1000</v>
-      </c>
-      <c r="I175">
-        <v>2</v>
-      </c>
-      <c r="J175">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>10</v>
-      </c>
-      <c r="B176">
-        <v>109</v>
-      </c>
-      <c r="C176" t="b">
-        <v>1</v>
-      </c>
-      <c r="D176" t="b">
-        <v>0</v>
-      </c>
-      <c r="E176">
-        <v>0.5</v>
-      </c>
-      <c r="F176">
-        <v>0.05</v>
-      </c>
-      <c r="G176" t="s">
-        <v>0</v>
-      </c>
-      <c r="H176">
-        <v>1000</v>
-      </c>
-      <c r="I176">
-        <v>2</v>
-      </c>
-      <c r="J176">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>10</v>
-      </c>
-      <c r="B177">
-        <v>110</v>
-      </c>
-      <c r="C177" t="b">
-        <v>1</v>
-      </c>
-      <c r="D177" t="b">
-        <v>0</v>
-      </c>
-      <c r="E177">
-        <v>0.5</v>
-      </c>
-      <c r="F177">
-        <v>0.05</v>
-      </c>
-      <c r="G177" t="s">
-        <v>0</v>
-      </c>
-      <c r="H177">
-        <v>1000</v>
-      </c>
-      <c r="I177">
-        <v>2</v>
-      </c>
-      <c r="J177">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>10</v>
-      </c>
-      <c r="B178">
-        <v>111</v>
-      </c>
-      <c r="C178" t="b">
-        <v>1</v>
-      </c>
-      <c r="D178" t="b">
-        <v>0</v>
-      </c>
-      <c r="E178">
-        <v>0.5</v>
-      </c>
-      <c r="F178">
-        <v>0.05</v>
-      </c>
-      <c r="G178" t="s">
-        <v>0</v>
-      </c>
-      <c r="H178">
-        <v>1000</v>
-      </c>
-      <c r="I178">
-        <v>2</v>
-      </c>
-      <c r="J178">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>10</v>
-      </c>
-      <c r="B179">
-        <v>112</v>
-      </c>
-      <c r="C179" t="b">
-        <v>1</v>
-      </c>
-      <c r="D179" t="b">
-        <v>0</v>
-      </c>
-      <c r="E179">
-        <v>0.5</v>
-      </c>
-      <c r="F179">
-        <v>0.05</v>
-      </c>
-      <c r="G179" t="s">
-        <v>0</v>
-      </c>
-      <c r="H179">
-        <v>1000</v>
-      </c>
-      <c r="I179">
-        <v>2</v>
-      </c>
-      <c r="J179">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>10</v>
-      </c>
-      <c r="B180">
-        <v>113</v>
-      </c>
-      <c r="C180" t="b">
-        <v>1</v>
-      </c>
-      <c r="D180" t="b">
-        <v>0</v>
-      </c>
-      <c r="E180">
-        <v>0.5</v>
-      </c>
-      <c r="F180">
-        <v>0.05</v>
-      </c>
-      <c r="G180" t="s">
-        <v>0</v>
-      </c>
-      <c r="H180">
-        <v>1000</v>
-      </c>
-      <c r="I180">
-        <v>2</v>
-      </c>
-      <c r="J180">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>10</v>
-      </c>
-      <c r="B181">
-        <v>114</v>
-      </c>
-      <c r="C181" t="b">
-        <v>1</v>
-      </c>
-      <c r="D181" t="b">
-        <v>0</v>
-      </c>
-      <c r="E181">
-        <v>0.5</v>
-      </c>
-      <c r="F181">
-        <v>0.05</v>
-      </c>
-      <c r="G181" t="s">
-        <v>0</v>
-      </c>
-      <c r="H181">
-        <v>1000</v>
-      </c>
-      <c r="I181">
-        <v>2</v>
-      </c>
-      <c r="J181">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>10</v>
-      </c>
-      <c r="B182">
-        <v>115</v>
-      </c>
-      <c r="C182" t="b">
-        <v>1</v>
-      </c>
-      <c r="D182" t="b">
-        <v>0</v>
-      </c>
-      <c r="E182">
-        <v>0.5</v>
-      </c>
-      <c r="F182">
-        <v>0.05</v>
-      </c>
-      <c r="G182" t="s">
-        <v>0</v>
-      </c>
-      <c r="H182">
-        <v>1000</v>
-      </c>
-      <c r="I182">
-        <v>2</v>
-      </c>
-      <c r="J182">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>10</v>
-      </c>
-      <c r="B183">
-        <v>116</v>
-      </c>
-      <c r="C183" t="b">
-        <v>1</v>
-      </c>
-      <c r="D183" t="b">
-        <v>0</v>
-      </c>
-      <c r="E183">
-        <v>0.5</v>
-      </c>
-      <c r="F183">
-        <v>0.05</v>
-      </c>
-      <c r="G183" t="s">
-        <v>0</v>
-      </c>
-      <c r="H183">
-        <v>1000</v>
-      </c>
-      <c r="I183">
-        <v>2</v>
-      </c>
-      <c r="J183">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>10</v>
-      </c>
-      <c r="B184">
-        <v>117</v>
-      </c>
-      <c r="C184" t="b">
-        <v>1</v>
-      </c>
-      <c r="D184" t="b">
-        <v>0</v>
-      </c>
-      <c r="E184">
-        <v>0.5</v>
-      </c>
-      <c r="F184">
-        <v>0.05</v>
-      </c>
-      <c r="G184" t="s">
-        <v>0</v>
-      </c>
-      <c r="H184">
-        <v>1000</v>
-      </c>
-      <c r="I184">
-        <v>2</v>
-      </c>
-      <c r="J184">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
-        <v>10</v>
-      </c>
-      <c r="B185">
-        <v>118</v>
-      </c>
-      <c r="C185" t="b">
-        <v>1</v>
-      </c>
-      <c r="D185" t="b">
-        <v>0</v>
-      </c>
-      <c r="E185">
-        <v>0.5</v>
-      </c>
-      <c r="F185">
-        <v>0.05</v>
-      </c>
-      <c r="G185" t="s">
-        <v>0</v>
-      </c>
-      <c r="H185">
-        <v>1000</v>
-      </c>
-      <c r="I185">
-        <v>2</v>
-      </c>
-      <c r="J185">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>10</v>
-      </c>
-      <c r="B186">
-        <v>119</v>
-      </c>
-      <c r="C186" t="b">
-        <v>1</v>
-      </c>
-      <c r="D186" t="b">
-        <v>0</v>
-      </c>
-      <c r="E186">
-        <v>0.5</v>
-      </c>
-      <c r="F186">
-        <v>0.05</v>
-      </c>
-      <c r="G186" t="s">
-        <v>0</v>
-      </c>
-      <c r="H186">
-        <v>1000</v>
-      </c>
-      <c r="I186">
-        <v>2</v>
-      </c>
-      <c r="J186">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>10</v>
-      </c>
-      <c r="B187">
-        <v>120</v>
-      </c>
-      <c r="C187" t="b">
-        <v>1</v>
-      </c>
-      <c r="D187" t="b">
-        <v>0</v>
-      </c>
-      <c r="E187">
-        <v>0.5</v>
-      </c>
-      <c r="F187">
-        <v>0.05</v>
-      </c>
-      <c r="G187" t="s">
-        <v>0</v>
-      </c>
-      <c r="H187">
-        <v>1000</v>
-      </c>
-      <c r="I187">
-        <v>2</v>
-      </c>
-      <c r="J187">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>10</v>
-      </c>
-      <c r="B188">
-        <v>121</v>
-      </c>
-      <c r="C188" t="b">
-        <v>1</v>
-      </c>
-      <c r="D188" t="b">
-        <v>0</v>
-      </c>
-      <c r="E188">
-        <v>0.5</v>
-      </c>
-      <c r="F188">
-        <v>0.05</v>
-      </c>
-      <c r="G188" t="s">
-        <v>0</v>
-      </c>
-      <c r="H188">
-        <v>1000</v>
-      </c>
-      <c r="I188">
-        <v>2</v>
-      </c>
-      <c r="J188">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>10</v>
-      </c>
-      <c r="B189">
-        <v>122</v>
-      </c>
-      <c r="C189" t="b">
-        <v>1</v>
-      </c>
-      <c r="D189" t="b">
-        <v>0</v>
-      </c>
-      <c r="E189">
-        <v>0.5</v>
-      </c>
-      <c r="F189">
-        <v>0.05</v>
-      </c>
-      <c r="G189" t="s">
-        <v>0</v>
-      </c>
-      <c r="H189">
-        <v>1000</v>
-      </c>
-      <c r="I189">
-        <v>2</v>
-      </c>
-      <c r="J189">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
-        <v>10</v>
-      </c>
-      <c r="B190">
-        <v>123</v>
-      </c>
-      <c r="C190" t="b">
-        <v>1</v>
-      </c>
-      <c r="D190" t="b">
-        <v>0</v>
-      </c>
-      <c r="E190">
-        <v>0.5</v>
-      </c>
-      <c r="F190">
-        <v>0.05</v>
-      </c>
-      <c r="G190" t="s">
-        <v>0</v>
-      </c>
-      <c r="H190">
-        <v>1000</v>
-      </c>
-      <c r="I190">
-        <v>2</v>
-      </c>
-      <c r="J190">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>10</v>
-      </c>
-      <c r="B191">
-        <v>124</v>
-      </c>
-      <c r="C191" t="b">
-        <v>1</v>
-      </c>
-      <c r="D191" t="b">
-        <v>0</v>
-      </c>
-      <c r="E191">
-        <v>0.5</v>
-      </c>
-      <c r="F191">
-        <v>0.05</v>
-      </c>
-      <c r="G191" t="s">
-        <v>0</v>
-      </c>
-      <c r="H191">
-        <v>1000</v>
-      </c>
-      <c r="I191">
-        <v>2</v>
-      </c>
-      <c r="J191">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>10</v>
-      </c>
-      <c r="B192">
-        <v>125</v>
-      </c>
-      <c r="C192" t="b">
-        <v>1</v>
-      </c>
-      <c r="D192" t="b">
-        <v>0</v>
-      </c>
-      <c r="E192">
-        <v>0.5</v>
-      </c>
-      <c r="F192">
-        <v>0.05</v>
-      </c>
-      <c r="G192" t="s">
-        <v>0</v>
-      </c>
-      <c r="H192">
-        <v>1000</v>
-      </c>
-      <c r="I192">
-        <v>2</v>
-      </c>
-      <c r="J192">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Back to 121 completed and change folder path a bit
</commit_message>
<xml_diff>
--- a/budgetq/nlp/train_params.xlsx
+++ b/budgetq/nlp/train_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/ppa/budgetq/nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24FD234-14C1-F84D-A899-0EF64BE4373B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F7F263-E1A0-1C43-81A5-8CD335BECE0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144:F152"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="M149" sqref="M149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F40">
         <v>0.1</v>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="F41">
         <v>0.1</v>
@@ -1735,7 +1735,7 @@
         <v>10</v>
       </c>
       <c r="B42">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C42" t="b">
         <v>1</v>
@@ -1744,7 +1744,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="F42">
         <v>0.1</v>
@@ -1767,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="B43">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -1799,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="B44">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -1831,7 +1831,7 @@
         <v>10</v>
       </c>
       <c r="B45">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -1863,7 +1863,7 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -1895,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="B47">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
@@ -1927,7 +1927,7 @@
         <v>10</v>
       </c>
       <c r="B48">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -1959,7 +1959,7 @@
         <v>10</v>
       </c>
       <c r="B49">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C49" t="b">
         <v>1</v>
@@ -1991,7 +1991,7 @@
         <v>10</v>
       </c>
       <c r="B50">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -2023,7 +2023,7 @@
         <v>10</v>
       </c>
       <c r="B51">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -2055,7 +2055,7 @@
         <v>10</v>
       </c>
       <c r="B52">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -2087,7 +2087,7 @@
         <v>10</v>
       </c>
       <c r="B53">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -2119,7 +2119,7 @@
         <v>10</v>
       </c>
       <c r="B54">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
@@ -2151,7 +2151,7 @@
         <v>10</v>
       </c>
       <c r="B55">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>10</v>
       </c>
       <c r="B56">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -2215,7 +2215,7 @@
         <v>10</v>
       </c>
       <c r="B57">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -2247,7 +2247,7 @@
         <v>10</v>
       </c>
       <c r="B58">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -2279,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="B59">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -2311,7 +2311,7 @@
         <v>10</v>
       </c>
       <c r="B60">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -2343,7 +2343,7 @@
         <v>10</v>
       </c>
       <c r="B61">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -2375,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="B62">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>10</v>
       </c>
       <c r="B63">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C63" t="b">
         <v>1</v>
@@ -2439,7 +2439,7 @@
         <v>10</v>
       </c>
       <c r="B64">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -2471,7 +2471,7 @@
         <v>10</v>
       </c>
       <c r="B65">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -2503,7 +2503,7 @@
         <v>10</v>
       </c>
       <c r="B66">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -2535,7 +2535,7 @@
         <v>10</v>
       </c>
       <c r="B67">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -2567,7 +2567,7 @@
         <v>10</v>
       </c>
       <c r="B68">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C68" t="b">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         <v>10</v>
       </c>
       <c r="B69">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -2631,7 +2631,7 @@
         <v>10</v>
       </c>
       <c r="B70">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -2663,7 +2663,7 @@
         <v>10</v>
       </c>
       <c r="B71">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -2695,7 +2695,7 @@
         <v>10</v>
       </c>
       <c r="B72">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -2727,7 +2727,7 @@
         <v>10</v>
       </c>
       <c r="B73">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -2759,7 +2759,7 @@
         <v>10</v>
       </c>
       <c r="B74">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -2791,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="B75">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -2823,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="B76">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>
@@ -2855,7 +2855,7 @@
         <v>10</v>
       </c>
       <c r="B77">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C77" t="b">
         <v>1</v>
@@ -2887,7 +2887,7 @@
         <v>10</v>
       </c>
       <c r="B78">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C78" t="b">
         <v>1</v>
@@ -2899,7 +2899,7 @@
         <v>0.5</v>
       </c>
       <c r="F78">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G78" t="s">
         <v>0</v>
@@ -2919,7 +2919,7 @@
         <v>10</v>
       </c>
       <c r="B79">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C79" t="b">
         <v>1</v>
@@ -2931,7 +2931,7 @@
         <v>0.5</v>
       </c>
       <c r="F79">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G79" t="s">
         <v>0</v>
@@ -2951,7 +2951,7 @@
         <v>10</v>
       </c>
       <c r="B80">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C80" t="b">
         <v>1</v>
@@ -2963,7 +2963,7 @@
         <v>0.5</v>
       </c>
       <c r="F80">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G80" t="s">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>10</v>
       </c>
       <c r="B81">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C81" t="b">
         <v>1</v>
@@ -2995,7 +2995,7 @@
         <v>0.5</v>
       </c>
       <c r="F81">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G81" t="s">
         <v>0</v>
@@ -3015,7 +3015,7 @@
         <v>10</v>
       </c>
       <c r="B82">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C82" t="b">
         <v>1</v>
@@ -3027,7 +3027,7 @@
         <v>0.5</v>
       </c>
       <c r="F82">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G82" t="s">
         <v>0</v>
@@ -3047,7 +3047,7 @@
         <v>10</v>
       </c>
       <c r="B83">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C83" t="b">
         <v>1</v>
@@ -3059,7 +3059,7 @@
         <v>0.5</v>
       </c>
       <c r="F83">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G83" t="s">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>10</v>
       </c>
       <c r="B84">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C84" t="b">
         <v>1</v>
@@ -3091,7 +3091,7 @@
         <v>0.5</v>
       </c>
       <c r="F84">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G84" t="s">
         <v>0</v>
@@ -3111,7 +3111,7 @@
         <v>10</v>
       </c>
       <c r="B85">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C85" t="b">
         <v>1</v>
@@ -3123,7 +3123,7 @@
         <v>0.5</v>
       </c>
       <c r="F85">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G85" t="s">
         <v>0</v>
@@ -3143,7 +3143,7 @@
         <v>10</v>
       </c>
       <c r="B86">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C86" t="b">
         <v>1</v>
@@ -3155,7 +3155,7 @@
         <v>0.5</v>
       </c>
       <c r="F86">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G86" t="s">
         <v>0</v>
@@ -3175,7 +3175,7 @@
         <v>10</v>
       </c>
       <c r="B87">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C87" t="b">
         <v>1</v>
@@ -3187,7 +3187,7 @@
         <v>0.5</v>
       </c>
       <c r="F87">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G87" t="s">
         <v>0</v>
@@ -3207,7 +3207,7 @@
         <v>10</v>
       </c>
       <c r="B88">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C88" t="b">
         <v>1</v>
@@ -3239,7 +3239,7 @@
         <v>10</v>
       </c>
       <c r="B89">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C89" t="b">
         <v>1</v>
@@ -3271,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="B90">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C90" t="b">
         <v>1</v>
@@ -3303,7 +3303,7 @@
         <v>10</v>
       </c>
       <c r="B91">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C91" t="b">
         <v>1</v>
@@ -3335,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="B92">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C92" t="b">
         <v>1</v>
@@ -3367,7 +3367,7 @@
         <v>10</v>
       </c>
       <c r="B93">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C93" t="b">
         <v>1</v>
@@ -3379,7 +3379,7 @@
         <v>0.5</v>
       </c>
       <c r="F93">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G93" t="s">
         <v>0</v>
@@ -3388,7 +3388,7 @@
         <v>1000</v>
       </c>
       <c r="I93">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J93">
         <v>20</v>
@@ -3399,7 +3399,7 @@
         <v>10</v>
       </c>
       <c r="B94">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C94" t="b">
         <v>1</v>
@@ -3411,7 +3411,7 @@
         <v>0.5</v>
       </c>
       <c r="F94">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G94" t="s">
         <v>0</v>
@@ -3420,7 +3420,7 @@
         <v>1000</v>
       </c>
       <c r="I94">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J94">
         <v>20</v>
@@ -3431,7 +3431,7 @@
         <v>10</v>
       </c>
       <c r="B95">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C95" t="b">
         <v>1</v>
@@ -3443,7 +3443,7 @@
         <v>0.5</v>
       </c>
       <c r="F95">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G95" t="s">
         <v>0</v>
@@ -3452,7 +3452,7 @@
         <v>1000</v>
       </c>
       <c r="I95">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J95">
         <v>20</v>
@@ -3463,7 +3463,7 @@
         <v>10</v>
       </c>
       <c r="B96">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C96" t="b">
         <v>1</v>
@@ -3475,7 +3475,7 @@
         <v>0.5</v>
       </c>
       <c r="F96">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G96" t="s">
         <v>0</v>
@@ -3484,7 +3484,7 @@
         <v>1000</v>
       </c>
       <c r="I96">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J96">
         <v>20</v>
@@ -3495,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="B97">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C97" t="b">
         <v>1</v>
@@ -3507,7 +3507,7 @@
         <v>0.5</v>
       </c>
       <c r="F97">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G97" t="s">
         <v>0</v>
@@ -3516,7 +3516,7 @@
         <v>1000</v>
       </c>
       <c r="I97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J97">
         <v>20</v>
@@ -3527,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="B98">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C98" t="b">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>0.5</v>
       </c>
       <c r="F98">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G98" t="s">
         <v>0</v>
@@ -3548,7 +3548,7 @@
         <v>1000</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J98">
         <v>20</v>
@@ -3559,7 +3559,7 @@
         <v>10</v>
       </c>
       <c r="B99">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C99" t="b">
         <v>1</v>
@@ -3571,7 +3571,7 @@
         <v>0.5</v>
       </c>
       <c r="F99">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G99" t="s">
         <v>0</v>
@@ -3580,7 +3580,7 @@
         <v>1000</v>
       </c>
       <c r="I99">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J99">
         <v>20</v>
@@ -3591,7 +3591,7 @@
         <v>10</v>
       </c>
       <c r="B100">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C100" t="b">
         <v>1</v>
@@ -3603,7 +3603,7 @@
         <v>0.5</v>
       </c>
       <c r="F100">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G100" t="s">
         <v>0</v>
@@ -3612,7 +3612,7 @@
         <v>1000</v>
       </c>
       <c r="I100">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J100">
         <v>20</v>
@@ -3623,7 +3623,7 @@
         <v>10</v>
       </c>
       <c r="B101">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C101" t="b">
         <v>1</v>
@@ -3635,7 +3635,7 @@
         <v>0.5</v>
       </c>
       <c r="F101">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G101" t="s">
         <v>0</v>
@@ -3644,7 +3644,7 @@
         <v>1000</v>
       </c>
       <c r="I101">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J101">
         <v>20</v>
@@ -3655,7 +3655,7 @@
         <v>10</v>
       </c>
       <c r="B102">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C102" t="b">
         <v>1</v>
@@ -3667,7 +3667,7 @@
         <v>0.5</v>
       </c>
       <c r="F102">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G102" t="s">
         <v>0</v>
@@ -3676,7 +3676,7 @@
         <v>1000</v>
       </c>
       <c r="I102">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J102">
         <v>20</v>
@@ -3687,7 +3687,7 @@
         <v>10</v>
       </c>
       <c r="B103">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C103" t="b">
         <v>1</v>
@@ -3708,7 +3708,7 @@
         <v>1000</v>
       </c>
       <c r="I103">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J103">
         <v>20</v>
@@ -3719,7 +3719,7 @@
         <v>10</v>
       </c>
       <c r="B104">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C104" t="b">
         <v>1</v>
@@ -3740,7 +3740,7 @@
         <v>1000</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J104">
         <v>20</v>
@@ -3751,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="B105">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C105" t="b">
         <v>1</v>
@@ -3772,7 +3772,7 @@
         <v>1000</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J105">
         <v>20</v>
@@ -3783,7 +3783,7 @@
         <v>10</v>
       </c>
       <c r="B106">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C106" t="b">
         <v>1</v>
@@ -3804,7 +3804,7 @@
         <v>1000</v>
       </c>
       <c r="I106">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J106">
         <v>20</v>
@@ -3815,7 +3815,7 @@
         <v>10</v>
       </c>
       <c r="B107">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C107" t="b">
         <v>1</v>
@@ -3836,7 +3836,7 @@
         <v>1000</v>
       </c>
       <c r="I107">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J107">
         <v>20</v>
@@ -3847,7 +3847,7 @@
         <v>10</v>
       </c>
       <c r="B108">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C108" t="b">
         <v>1</v>
@@ -3868,7 +3868,7 @@
         <v>1000</v>
       </c>
       <c r="I108">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J108">
         <v>20</v>
@@ -3879,7 +3879,7 @@
         <v>10</v>
       </c>
       <c r="B109">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C109" t="b">
         <v>1</v>
@@ -3900,7 +3900,7 @@
         <v>1000</v>
       </c>
       <c r="I109">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J109">
         <v>20</v>
@@ -3911,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="B110">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C110" t="b">
         <v>1</v>
@@ -3932,7 +3932,7 @@
         <v>1000</v>
       </c>
       <c r="I110">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J110">
         <v>20</v>
@@ -3943,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="B111">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C111" t="b">
         <v>1</v>
@@ -3964,7 +3964,7 @@
         <v>1000</v>
       </c>
       <c r="I111">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J111">
         <v>20</v>
@@ -3975,7 +3975,7 @@
         <v>10</v>
       </c>
       <c r="B112">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C112" t="b">
         <v>1</v>
@@ -3996,7 +3996,7 @@
         <v>1000</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J112">
         <v>20</v>
@@ -4019,7 +4019,7 @@
         <v>0.5</v>
       </c>
       <c r="F113">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G113" t="s">
         <v>0</v>
@@ -4028,7 +4028,7 @@
         <v>1000</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J113">
         <v>20</v>
@@ -4051,7 +4051,7 @@
         <v>0.5</v>
       </c>
       <c r="F114">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G114" t="s">
         <v>0</v>
@@ -4060,7 +4060,7 @@
         <v>1000</v>
       </c>
       <c r="I114">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J114">
         <v>20</v>
@@ -4083,7 +4083,7 @@
         <v>0.5</v>
       </c>
       <c r="F115">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G115" t="s">
         <v>0</v>
@@ -4092,7 +4092,7 @@
         <v>1000</v>
       </c>
       <c r="I115">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J115">
         <v>20</v>
@@ -4115,7 +4115,7 @@
         <v>0.5</v>
       </c>
       <c r="F116">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G116" t="s">
         <v>0</v>
@@ -4124,7 +4124,7 @@
         <v>1000</v>
       </c>
       <c r="I116">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J116">
         <v>20</v>
@@ -4147,7 +4147,7 @@
         <v>0.5</v>
       </c>
       <c r="F117">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G117" t="s">
         <v>0</v>
@@ -4156,7 +4156,7 @@
         <v>1000</v>
       </c>
       <c r="I117">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J117">
         <v>20</v>
@@ -4179,7 +4179,7 @@
         <v>0.5</v>
       </c>
       <c r="F118">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G118" t="s">
         <v>0</v>
@@ -4188,7 +4188,7 @@
         <v>1000</v>
       </c>
       <c r="I118">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J118">
         <v>20</v>
@@ -4211,7 +4211,7 @@
         <v>0.5</v>
       </c>
       <c r="F119">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G119" t="s">
         <v>0</v>
@@ -4220,7 +4220,7 @@
         <v>1000</v>
       </c>
       <c r="I119">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J119">
         <v>20</v>
@@ -4243,7 +4243,7 @@
         <v>0.5</v>
       </c>
       <c r="F120">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G120" t="s">
         <v>0</v>
@@ -4252,7 +4252,7 @@
         <v>1000</v>
       </c>
       <c r="I120">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J120">
         <v>20</v>
@@ -4275,7 +4275,7 @@
         <v>0.5</v>
       </c>
       <c r="F121">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G121" t="s">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>1000</v>
       </c>
       <c r="I121">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J121">
         <v>20</v>
@@ -4307,7 +4307,7 @@
         <v>0.5</v>
       </c>
       <c r="F122">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G122" t="s">
         <v>0</v>
@@ -4316,7 +4316,7 @@
         <v>1000</v>
       </c>
       <c r="I122">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J122">
         <v>20</v>
@@ -4339,7 +4339,7 @@
         <v>0.5</v>
       </c>
       <c r="F123">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G123" t="s">
         <v>0</v>
@@ -4348,7 +4348,7 @@
         <v>1000</v>
       </c>
       <c r="I123">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J123">
         <v>20</v>
@@ -4371,7 +4371,7 @@
         <v>0.5</v>
       </c>
       <c r="F124">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G124" t="s">
         <v>0</v>
@@ -4380,7 +4380,7 @@
         <v>1000</v>
       </c>
       <c r="I124">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J124">
         <v>20</v>
@@ -4403,7 +4403,7 @@
         <v>0.5</v>
       </c>
       <c r="F125">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G125" t="s">
         <v>0</v>
@@ -4412,7 +4412,7 @@
         <v>1000</v>
       </c>
       <c r="I125">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J125">
         <v>20</v>
@@ -4435,7 +4435,7 @@
         <v>0.5</v>
       </c>
       <c r="F126">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G126" t="s">
         <v>0</v>
@@ -4444,7 +4444,7 @@
         <v>1000</v>
       </c>
       <c r="I126">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J126">
         <v>20</v>
@@ -4467,7 +4467,7 @@
         <v>0.5</v>
       </c>
       <c r="F127">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G127" t="s">
         <v>0</v>
@@ -4476,7 +4476,7 @@
         <v>1000</v>
       </c>
       <c r="I127">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J127">
         <v>20</v>
@@ -4499,7 +4499,7 @@
         <v>0.5</v>
       </c>
       <c r="F128">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G128" t="s">
         <v>0</v>
@@ -4508,7 +4508,7 @@
         <v>1000</v>
       </c>
       <c r="I128">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J128">
         <v>20</v>
@@ -4531,7 +4531,7 @@
         <v>0.5</v>
       </c>
       <c r="F129">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G129" t="s">
         <v>0</v>
@@ -4540,7 +4540,7 @@
         <v>1000</v>
       </c>
       <c r="I129">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J129">
         <v>20</v>
@@ -4563,7 +4563,7 @@
         <v>0.5</v>
       </c>
       <c r="F130">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G130" t="s">
         <v>0</v>
@@ -4572,7 +4572,7 @@
         <v>1000</v>
       </c>
       <c r="I130">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J130">
         <v>20</v>
@@ -4595,7 +4595,7 @@
         <v>0.5</v>
       </c>
       <c r="F131">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G131" t="s">
         <v>0</v>
@@ -4604,7 +4604,7 @@
         <v>1000</v>
       </c>
       <c r="I131">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J131">
         <v>20</v>
@@ -4627,7 +4627,7 @@
         <v>0.5</v>
       </c>
       <c r="F132">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="G132" t="s">
         <v>0</v>
@@ -4636,7 +4636,7 @@
         <v>1000</v>
       </c>
       <c r="I132">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J132">
         <v>20</v>
@@ -4668,7 +4668,7 @@
         <v>1000</v>
       </c>
       <c r="I133">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J133">
         <v>20</v>
@@ -4700,7 +4700,7 @@
         <v>1000</v>
       </c>
       <c r="I134">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J134">
         <v>20</v>
@@ -4732,7 +4732,7 @@
         <v>1000</v>
       </c>
       <c r="I135">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J135">
         <v>20</v>
@@ -4764,7 +4764,7 @@
         <v>1000</v>
       </c>
       <c r="I136">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J136">
         <v>20</v>
@@ -4796,7 +4796,7 @@
         <v>1000</v>
       </c>
       <c r="I137">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J137">
         <v>20</v>
@@ -4828,7 +4828,7 @@
         <v>1000</v>
       </c>
       <c r="I138">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J138">
         <v>20</v>
@@ -4860,7 +4860,7 @@
         <v>1000</v>
       </c>
       <c r="I139">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J139">
         <v>20</v>
@@ -4892,7 +4892,7 @@
         <v>1000</v>
       </c>
       <c r="I140">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J140">
         <v>20</v>
@@ -4924,7 +4924,7 @@
         <v>1000</v>
       </c>
       <c r="I141">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J141">
         <v>20</v>
@@ -4956,7 +4956,7 @@
         <v>1000</v>
       </c>
       <c r="I142">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J142">
         <v>20</v>
@@ -4979,7 +4979,7 @@
         <v>0.5</v>
       </c>
       <c r="F143">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G143" t="s">
         <v>0</v>
@@ -4988,7 +4988,7 @@
         <v>1000</v>
       </c>
       <c r="I143">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J143">
         <v>20</v>
@@ -5011,7 +5011,7 @@
         <v>0.5</v>
       </c>
       <c r="F144">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G144" t="s">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         <v>1000</v>
       </c>
       <c r="I144">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J144">
         <v>20</v>
@@ -5043,7 +5043,7 @@
         <v>0.5</v>
       </c>
       <c r="F145">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G145" t="s">
         <v>0</v>
@@ -5052,7 +5052,7 @@
         <v>1000</v>
       </c>
       <c r="I145">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J145">
         <v>20</v>
@@ -5075,7 +5075,7 @@
         <v>0.5</v>
       </c>
       <c r="F146">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G146" t="s">
         <v>0</v>
@@ -5084,7 +5084,7 @@
         <v>1000</v>
       </c>
       <c r="I146">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J146">
         <v>20</v>
@@ -5107,7 +5107,7 @@
         <v>0.5</v>
       </c>
       <c r="F147">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G147" t="s">
         <v>0</v>
@@ -5116,7 +5116,7 @@
         <v>1000</v>
       </c>
       <c r="I147">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J147">
         <v>20</v>
@@ -5139,7 +5139,7 @@
         <v>0.5</v>
       </c>
       <c r="F148">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G148" t="s">
         <v>0</v>
@@ -5148,7 +5148,7 @@
         <v>1000</v>
       </c>
       <c r="I148">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J148">
         <v>20</v>
@@ -5171,7 +5171,7 @@
         <v>0.5</v>
       </c>
       <c r="F149">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G149" t="s">
         <v>0</v>
@@ -5180,7 +5180,7 @@
         <v>1000</v>
       </c>
       <c r="I149">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J149">
         <v>20</v>
@@ -5203,7 +5203,7 @@
         <v>0.5</v>
       </c>
       <c r="F150">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G150" t="s">
         <v>0</v>
@@ -5212,7 +5212,7 @@
         <v>1000</v>
       </c>
       <c r="I150">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J150">
         <v>20</v>
@@ -5235,7 +5235,7 @@
         <v>0.5</v>
       </c>
       <c r="F151">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G151" t="s">
         <v>0</v>
@@ -5244,7 +5244,7 @@
         <v>1000</v>
       </c>
       <c r="I151">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J151">
         <v>20</v>
@@ -5267,7 +5267,7 @@
         <v>0.5</v>
       </c>
       <c r="F152">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G152" t="s">
         <v>0</v>
@@ -5276,7 +5276,7 @@
         <v>1000</v>
       </c>
       <c r="I152">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J152">
         <v>20</v>

</xml_diff>